<commit_message>
Work on logo animation, mockups
</commit_message>
<xml_diff>
--- a/Resources and Other Documents/Logo/Animated Logo/Timing Worksheet.xlsx
+++ b/Resources and Other Documents/Logo/Animated Logo/Timing Worksheet.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cyham\Documents\Personal-Website\Resources and Other Documents\Logo\Animated Logo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EEE1339-2DD6-4CA6-B480-40146AE0A096}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D02F154F-921B-47D6-B4DA-6AD367DE4D12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Timeline" sheetId="3" r:id="rId3"/>
+    <sheet name="Attempt 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Attempt 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Once" sheetId="4" r:id="rId3"/>
+    <sheet name="Timeline" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="52">
   <si>
     <t>Caroline</t>
   </si>
@@ -200,8 +201,8 @@
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
-    <numFmt numFmtId="167" formatCode="0.000%"/>
-    <numFmt numFmtId="172" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.000%"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -289,28 +290,28 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1593,15 +1594,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11C931AF-84BB-46A6-94D2-04793AD7EDFC}">
   <dimension ref="A1:Y30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView topLeftCell="F16" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.6640625" customWidth="1"/>
     <col min="2" max="4" width="30.5546875" customWidth="1"/>
-    <col min="5" max="5" width="30.5546875" style="16" customWidth="1"/>
+    <col min="5" max="5" width="30.5546875" style="12" customWidth="1"/>
     <col min="6" max="6" width="29.77734375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1613,19 +1614,19 @@
         <f>CONCATENATE(A1,"Animation")</f>
         <v>FirstLineAnimation</v>
       </c>
-      <c r="C1" s="16">
+      <c r="C1" s="12">
         <f>Timeline!B9</f>
         <v>5.4054054054054057E-2</v>
       </c>
-      <c r="D1" s="16">
+      <c r="D1" s="12">
         <f>Timeline!B65</f>
         <v>0.43243243243243246</v>
       </c>
-      <c r="E1" s="18">
+      <c r="E1" s="14">
         <f>C1*100</f>
         <v>5.4054054054054053</v>
       </c>
-      <c r="F1" s="20">
+      <c r="F1" s="16">
         <f>D1*100</f>
         <v>43.243243243243242</v>
       </c>
@@ -1646,24 +1647,24 @@
         <f t="shared" ref="B2:B13" si="0">CONCATENATE(A2,"Animation")</f>
         <v>CarolineAnimation</v>
       </c>
-      <c r="C2" s="16">
+      <c r="C2" s="12">
         <f>Timeline!B11</f>
         <v>6.7567567567567571E-2</v>
       </c>
-      <c r="D2" s="16">
+      <c r="D2" s="12">
         <f>Timeline!B63</f>
         <v>0.41891891891891891</v>
       </c>
-      <c r="E2" s="18">
+      <c r="E2" s="14">
         <f t="shared" ref="E2:E30" si="1">C2*100</f>
         <v>6.756756756756757</v>
       </c>
-      <c r="F2" s="20">
+      <c r="F2" s="16">
         <f t="shared" ref="F2:F30" si="2">D2*100</f>
         <v>41.891891891891895</v>
       </c>
       <c r="G2" t="str">
-        <f t="shared" ref="G2:G13" si="3">CONCATENATE("@keyframes ",B2, " { 0%, ",ROUND(E2,3)- 0.001, "% {opacity: 0} ",ROUND(E2,3), "%, ",ROUND(E3,3)-0.001, "% {opacity: 1} ", ROUND(E3,3), "%, ", ROUND(F2, 3)-0.001,"% {opacity: 0} ", ROUND(F2, 3),"%, ", ROUND(F1, 3)-0.001,"% {opacity: 1 } ", ROUND(F1, 3), "%, 100% {opacity: 0} }")</f>
+        <f t="shared" ref="G2:G12" si="3">CONCATENATE("@keyframes ",B2, " { 0%, ",ROUND(E2,3)- 0.001, "% {opacity: 0} ",ROUND(E2,3), "%, ",ROUND(E3,3)-0.001, "% {opacity: 1} ", ROUND(E3,3), "%, ", ROUND(F2, 3)-0.001,"% {opacity: 0} ", ROUND(F2, 3),"%, ", ROUND(F1, 3)-0.001,"% {opacity: 1 } ", ROUND(F1, 3), "%, 100% {opacity: 0} }")</f>
         <v>@keyframes CarolineAnimation { 0%, 6.756% {opacity: 0} 6.757%, 8.107% {opacity: 1} 8.108%, 41.891% {opacity: 0} 41.892%, 43.242% {opacity: 1 } 43.243%, 100% {opacity: 0} }</v>
       </c>
       <c r="H2" s="9"/>
@@ -1680,19 +1681,19 @@
         <f t="shared" si="0"/>
         <v>CAroline2Animation</v>
       </c>
-      <c r="C3" s="16">
+      <c r="C3" s="12">
         <f>Timeline!B13</f>
         <v>8.1081081081081086E-2</v>
       </c>
-      <c r="D3" s="16">
+      <c r="D3" s="12">
         <f>Timeline!B61</f>
         <v>0.40540540540540543</v>
       </c>
-      <c r="E3" s="18">
-        <f>C3*100</f>
+      <c r="E3" s="14">
+        <f t="shared" ref="E3:E9" si="5">C3*100</f>
         <v>8.1081081081081088</v>
       </c>
-      <c r="F3" s="19">
+      <c r="F3" s="15">
         <f t="shared" si="2"/>
         <v>40.54054054054054</v>
       </c>
@@ -1713,19 +1714,19 @@
         <f t="shared" si="0"/>
         <v>CARoline3Animation</v>
       </c>
-      <c r="C4" s="16">
+      <c r="C4" s="12">
         <f>Timeline!B15</f>
         <v>9.45945945945946E-2</v>
       </c>
-      <c r="D4" s="16">
+      <c r="D4" s="12">
         <f>Timeline!B59</f>
         <v>0.39189189189189189</v>
       </c>
-      <c r="E4" s="18">
-        <f>C4*100</f>
+      <c r="E4" s="14">
+        <f t="shared" si="5"/>
         <v>9.4594594594594597</v>
       </c>
-      <c r="F4" s="19">
+      <c r="F4" s="15">
         <f t="shared" si="2"/>
         <v>39.189189189189186</v>
       </c>
@@ -1746,19 +1747,19 @@
         <f t="shared" si="0"/>
         <v>CAROline4Animation</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="12">
         <f>Timeline!B17</f>
         <v>0.10810810810810811</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5" s="12">
         <f>Timeline!B57</f>
         <v>0.3783783783783784</v>
       </c>
-      <c r="E5" s="18">
-        <f>C5*100</f>
+      <c r="E5" s="14">
+        <f t="shared" si="5"/>
         <v>10.810810810810811</v>
       </c>
-      <c r="F5" s="19">
+      <c r="F5" s="15">
         <f t="shared" si="2"/>
         <v>37.837837837837839</v>
       </c>
@@ -1779,19 +1780,19 @@
         <f t="shared" si="0"/>
         <v>CAROLine5Animation</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6" s="12">
         <f>Timeline!B19</f>
         <v>0.12162162162162163</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D6" s="12">
         <f>Timeline!B55</f>
         <v>0.36486486486486486</v>
       </c>
-      <c r="E6" s="18">
-        <f>C6*100</f>
+      <c r="E6" s="14">
+        <f t="shared" si="5"/>
         <v>12.162162162162163</v>
       </c>
-      <c r="F6" s="19">
+      <c r="F6" s="15">
         <f t="shared" si="2"/>
         <v>36.486486486486484</v>
       </c>
@@ -1812,19 +1813,19 @@
         <f t="shared" si="0"/>
         <v>CAROLIne6Animation</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="12">
         <f>Timeline!B21</f>
         <v>0.13513513513513514</v>
       </c>
-      <c r="D7" s="16">
+      <c r="D7" s="12">
         <f>Timeline!B53</f>
         <v>0.35135135135135137</v>
       </c>
-      <c r="E7" s="18">
-        <f>C7*100</f>
+      <c r="E7" s="14">
+        <f t="shared" si="5"/>
         <v>13.513513513513514</v>
       </c>
-      <c r="F7" s="19">
+      <c r="F7" s="15">
         <f t="shared" si="2"/>
         <v>35.135135135135137</v>
       </c>
@@ -1845,19 +1846,19 @@
         <f t="shared" si="0"/>
         <v>CAROLINe7Animation</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C8" s="12">
         <f>Timeline!B23</f>
         <v>0.14864864864864866</v>
       </c>
-      <c r="D8" s="16">
+      <c r="D8" s="12">
         <f>Timeline!B51</f>
         <v>0.33783783783783783</v>
       </c>
-      <c r="E8" s="18">
-        <f>C8*100</f>
+      <c r="E8" s="14">
+        <f t="shared" si="5"/>
         <v>14.864864864864865</v>
       </c>
-      <c r="F8" s="19">
+      <c r="F8" s="15">
         <f t="shared" si="2"/>
         <v>33.783783783783782</v>
       </c>
@@ -1878,19 +1879,19 @@
         <f t="shared" si="0"/>
         <v>CAROLINE8Animation</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="12">
         <f>Timeline!B25</f>
         <v>0.16216216216216217</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="12">
         <f>Timeline!B49</f>
         <v>0.32432432432432434</v>
       </c>
-      <c r="E9" s="18">
-        <f>C9*100</f>
+      <c r="E9" s="14">
+        <f t="shared" si="5"/>
         <v>16.216216216216218</v>
       </c>
-      <c r="F9" s="19">
+      <c r="F9" s="15">
         <f t="shared" si="2"/>
         <v>32.432432432432435</v>
       </c>
@@ -1911,19 +1912,19 @@
         <f t="shared" si="0"/>
         <v>CAROLINE_SpaceAnimation</v>
       </c>
-      <c r="C10" s="16">
+      <c r="C10" s="12">
         <f>Timeline!B27</f>
         <v>0.17567567567567569</v>
       </c>
-      <c r="D10" s="16">
+      <c r="D10" s="12">
         <f>Timeline!B47</f>
         <v>0.3108108108108108</v>
       </c>
-      <c r="E10" s="18">
+      <c r="E10" s="14">
         <f t="shared" si="1"/>
         <v>17.567567567567568</v>
       </c>
-      <c r="F10" s="19">
+      <c r="F10" s="15">
         <f t="shared" si="2"/>
         <v>31.081081081081081</v>
       </c>
@@ -1944,19 +1945,19 @@
         <f t="shared" si="0"/>
         <v>CAROLINE_HamAnimation</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="12">
         <f>Timeline!B29</f>
         <v>0.1891891891891892</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D11" s="12">
         <f>Timeline!B45</f>
         <v>0.29729729729729731</v>
       </c>
-      <c r="E11" s="18">
+      <c r="E11" s="14">
         <f t="shared" si="1"/>
         <v>18.918918918918919</v>
       </c>
-      <c r="F11" s="19">
+      <c r="F11" s="15">
         <f t="shared" si="2"/>
         <v>29.72972972972973</v>
       </c>
@@ -1977,19 +1978,19 @@
         <f t="shared" si="0"/>
         <v>CAROLINE_HAm2Animation</v>
       </c>
-      <c r="C12" s="16">
+      <c r="C12" s="12">
         <f>Timeline!B31</f>
         <v>0.20270270270270271</v>
       </c>
-      <c r="D12" s="16">
+      <c r="D12" s="12">
         <f>Timeline!B43</f>
         <v>0.28378378378378377</v>
       </c>
-      <c r="E12" s="18">
+      <c r="E12" s="14">
         <f t="shared" si="1"/>
         <v>20.27027027027027</v>
       </c>
-      <c r="F12" s="19">
+      <c r="F12" s="15">
         <f t="shared" si="2"/>
         <v>28.378378378378379</v>
       </c>
@@ -2010,19 +2011,19 @@
         <f t="shared" si="0"/>
         <v>CAROLINE_HAM3Animation</v>
       </c>
-      <c r="C13" s="16">
+      <c r="C13" s="12">
         <f>Timeline!B33</f>
         <v>0.21621621621621623</v>
       </c>
-      <c r="D13" s="16">
+      <c r="D13" s="12">
         <f>Timeline!B43</f>
         <v>0.28378378378378377</v>
       </c>
-      <c r="E13" s="18">
+      <c r="E13" s="14">
         <f t="shared" si="1"/>
         <v>21.621621621621621</v>
       </c>
-      <c r="F13" s="20">
+      <c r="F13" s="16">
         <f t="shared" si="2"/>
         <v>28.378378378378379</v>
       </c>
@@ -2040,22 +2041,22 @@
         <v>1</v>
       </c>
       <c r="B14" t="str">
-        <f>CONCATENATE(A14,"Animation")</f>
+        <f t="shared" ref="B14:B30" si="6">CONCATENATE(A14,"Animation")</f>
         <v>SoftwareAnimation</v>
       </c>
-      <c r="C14" s="16">
+      <c r="C14" s="12">
         <f>Timeline!B75</f>
         <v>0.5</v>
       </c>
-      <c r="D14" s="16">
+      <c r="D14" s="12">
         <f>Timeline!B147</f>
         <v>0.98648648648648651</v>
       </c>
-      <c r="E14" s="18">
+      <c r="E14" s="14">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="F14" s="20">
+      <c r="F14" s="16">
         <f t="shared" si="2"/>
         <v>98.648648648648646</v>
       </c>
@@ -2073,22 +2074,22 @@
         <v>13</v>
       </c>
       <c r="B15" t="str">
-        <f>CONCATENATE(A15,"Animation")</f>
+        <f t="shared" si="6"/>
         <v>SOftware2Animation</v>
       </c>
-      <c r="C15" s="16">
+      <c r="C15" s="12">
         <f>Timeline!B77</f>
         <v>0.51351351351351349</v>
       </c>
-      <c r="D15" s="16">
+      <c r="D15" s="12">
         <f>Timeline!B145</f>
         <v>0.97297297297297303</v>
       </c>
-      <c r="E15" s="18">
+      <c r="E15" s="14">
         <f t="shared" si="1"/>
         <v>51.351351351351347</v>
       </c>
-      <c r="F15" s="21">
+      <c r="F15" s="17">
         <f t="shared" si="2"/>
         <v>97.297297297297305</v>
       </c>
@@ -2106,22 +2107,22 @@
         <v>14</v>
       </c>
       <c r="B16" t="str">
-        <f>CONCATENATE(A16,"Animation")</f>
+        <f t="shared" si="6"/>
         <v>SOFtware3Animation</v>
       </c>
-      <c r="C16" s="16">
+      <c r="C16" s="12">
         <f>Timeline!B79</f>
         <v>0.52702702702702697</v>
       </c>
-      <c r="D16" s="16">
+      <c r="D16" s="12">
         <f>Timeline!B143</f>
         <v>0.95945945945945943</v>
       </c>
-      <c r="E16" s="18">
+      <c r="E16" s="14">
         <f t="shared" si="1"/>
         <v>52.702702702702695</v>
       </c>
-      <c r="F16" s="19">
+      <c r="F16" s="15">
         <f t="shared" si="2"/>
         <v>95.945945945945937</v>
       </c>
@@ -2139,27 +2140,27 @@
         <v>15</v>
       </c>
       <c r="B17" t="str">
-        <f>CONCATENATE(A17,"Animation")</f>
+        <f t="shared" si="6"/>
         <v>SOFTware4Animation</v>
       </c>
-      <c r="C17" s="16">
+      <c r="C17" s="12">
         <f>Timeline!B81</f>
         <v>0.54054054054054057</v>
       </c>
-      <c r="D17" s="16">
+      <c r="D17" s="12">
         <f>Timeline!B141</f>
         <v>0.94594594594594594</v>
       </c>
-      <c r="E17" s="18">
+      <c r="E17" s="14">
         <f t="shared" si="1"/>
         <v>54.054054054054056</v>
       </c>
-      <c r="F17" s="19">
+      <c r="F17" s="15">
         <f t="shared" si="2"/>
         <v>94.594594594594597</v>
       </c>
       <c r="G17" t="str">
-        <f t="shared" ref="G17:G29" si="5">CONCATENATE("@keyframes ",B17, " { 0%, ",ROUND(E17,3)- 0.001, "% {opacity: 0} ",ROUND(E17,3), "%, ",ROUND(E18,3)-0.001, "% {opacity: 1} ", ROUND(E18,3), "%, ", ROUND(F17, 3)-0.001,"% {opacity: 0} ", ROUND(F17, 3),"%, ", ROUND(F16, 3)-0.001,"% {opacity: 1 } ", ROUND(F16, 3), "%, 100% {opacity: 0} }")</f>
+        <f t="shared" ref="G17:G29" si="7">CONCATENATE("@keyframes ",B17, " { 0%, ",ROUND(E17,3)- 0.001, "% {opacity: 0} ",ROUND(E17,3), "%, ",ROUND(E18,3)-0.001, "% {opacity: 1} ", ROUND(E18,3), "%, ", ROUND(F17, 3)-0.001,"% {opacity: 0} ", ROUND(F17, 3),"%, ", ROUND(F16, 3)-0.001,"% {opacity: 1 } ", ROUND(F16, 3), "%, 100% {opacity: 0} }")</f>
         <v>@keyframes SOFTware4Animation { 0%, 54.053% {opacity: 0} 54.054%, 55.404% {opacity: 1} 55.405%, 94.594% {opacity: 0} 94.595%, 95.945% {opacity: 1 } 95.946%, 100% {opacity: 0} }</v>
       </c>
       <c r="Y17" t="str">
@@ -2172,27 +2173,27 @@
         <v>16</v>
       </c>
       <c r="B18" t="str">
-        <f>CONCATENATE(A18,"Animation")</f>
+        <f t="shared" si="6"/>
         <v>SOFTWare5Animation</v>
       </c>
-      <c r="C18" s="16">
+      <c r="C18" s="12">
         <f>Timeline!B83</f>
         <v>0.55405405405405406</v>
       </c>
-      <c r="D18" s="16">
+      <c r="D18" s="12">
         <f>Timeline!B139</f>
         <v>0.93243243243243246</v>
       </c>
-      <c r="E18" s="18">
+      <c r="E18" s="14">
         <f t="shared" si="1"/>
         <v>55.405405405405403</v>
       </c>
-      <c r="F18" s="19">
+      <c r="F18" s="15">
         <f t="shared" si="2"/>
         <v>93.243243243243242</v>
       </c>
       <c r="G18" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>@keyframes SOFTWare5Animation { 0%, 55.404% {opacity: 0} 55.405%, 56.756% {opacity: 1} 56.757%, 93.242% {opacity: 0} 93.243%, 94.594% {opacity: 1 } 94.595%, 100% {opacity: 0} }</v>
       </c>
       <c r="Y18" t="str">
@@ -2205,27 +2206,27 @@
         <v>17</v>
       </c>
       <c r="B19" t="str">
-        <f>CONCATENATE(A19,"Animation")</f>
+        <f t="shared" si="6"/>
         <v>SOFTWAre6Animation</v>
       </c>
-      <c r="C19" s="16">
+      <c r="C19" s="12">
         <f>Timeline!B85</f>
         <v>0.56756756756756754</v>
       </c>
-      <c r="D19" s="16">
+      <c r="D19" s="12">
         <f>Timeline!B137</f>
         <v>0.91891891891891897</v>
       </c>
-      <c r="E19" s="18">
+      <c r="E19" s="14">
         <f t="shared" si="1"/>
         <v>56.756756756756758</v>
       </c>
-      <c r="F19" s="19">
+      <c r="F19" s="15">
         <f t="shared" si="2"/>
         <v>91.891891891891902</v>
       </c>
       <c r="G19" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>@keyframes SOFTWAre6Animation { 0%, 56.756% {opacity: 0} 56.757%, 58.107% {opacity: 1} 58.108%, 91.891% {opacity: 0} 91.892%, 93.242% {opacity: 1 } 93.243%, 100% {opacity: 0} }</v>
       </c>
       <c r="Y19" t="str">
@@ -2238,27 +2239,27 @@
         <v>18</v>
       </c>
       <c r="B20" t="str">
-        <f>CONCATENATE(A20,"Animation")</f>
+        <f t="shared" si="6"/>
         <v>SOFTWARe7Animation</v>
       </c>
-      <c r="C20" s="16">
+      <c r="C20" s="12">
         <f>Timeline!B87</f>
         <v>0.58108108108108103</v>
       </c>
-      <c r="D20" s="16">
+      <c r="D20" s="12">
         <f>Timeline!B135</f>
         <v>0.90540540540540537</v>
       </c>
-      <c r="E20" s="18">
+      <c r="E20" s="14">
         <f t="shared" si="1"/>
         <v>58.108108108108105</v>
       </c>
-      <c r="F20" s="19">
+      <c r="F20" s="15">
         <f t="shared" si="2"/>
         <v>90.540540540540533</v>
       </c>
       <c r="G20" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>@keyframes SOFTWARe7Animation { 0%, 58.107% {opacity: 0} 58.108%, 59.458% {opacity: 1} 59.459%, 90.54% {opacity: 0} 90.541%, 91.891% {opacity: 1 } 91.892%, 100% {opacity: 0} }</v>
       </c>
       <c r="Y20" t="str">
@@ -2271,27 +2272,27 @@
         <v>19</v>
       </c>
       <c r="B21" t="str">
-        <f>CONCATENATE(A21,"Animation")</f>
+        <f t="shared" si="6"/>
         <v>SOFTWARE8Animation</v>
       </c>
-      <c r="C21" s="16">
+      <c r="C21" s="12">
         <f>Timeline!B89</f>
         <v>0.59459459459459463</v>
       </c>
-      <c r="D21" s="16">
+      <c r="D21" s="12">
         <f>Timeline!B133</f>
         <v>0.89189189189189189</v>
       </c>
-      <c r="E21" s="18">
+      <c r="E21" s="14">
         <f t="shared" si="1"/>
         <v>59.45945945945946</v>
       </c>
-      <c r="F21" s="19">
+      <c r="F21" s="15">
         <f t="shared" si="2"/>
         <v>89.189189189189193</v>
       </c>
       <c r="G21" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>@keyframes SOFTWARE8Animation { 0%, 59.458% {opacity: 0} 59.459%, 60.81% {opacity: 1} 60.811%, 89.188% {opacity: 0} 89.189%, 90.54% {opacity: 1 } 90.541%, 100% {opacity: 0} }</v>
       </c>
       <c r="Y21" t="str">
@@ -2304,27 +2305,27 @@
         <v>20</v>
       </c>
       <c r="B22" t="str">
-        <f>CONCATENATE(A22,"Animation")</f>
+        <f t="shared" si="6"/>
         <v>SOFTWARE_SpaceAnimation</v>
       </c>
-      <c r="C22" s="16">
+      <c r="C22" s="12">
         <f>Timeline!B91</f>
         <v>0.60810810810810811</v>
       </c>
-      <c r="D22" s="16">
+      <c r="D22" s="12">
         <f>Timeline!B131</f>
         <v>0.8783783783783784</v>
       </c>
-      <c r="E22" s="18">
+      <c r="E22" s="14">
         <f t="shared" si="1"/>
         <v>60.810810810810814</v>
       </c>
-      <c r="F22" s="19">
+      <c r="F22" s="15">
         <f t="shared" si="2"/>
         <v>87.837837837837839</v>
       </c>
       <c r="G22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>@keyframes SOFTWARE_SpaceAnimation { 0%, 60.81% {opacity: 0} 60.811%, 62.161% {opacity: 1} 62.162%, 87.837% {opacity: 0} 87.838%, 89.188% {opacity: 1 } 89.189%, 100% {opacity: 0} }</v>
       </c>
       <c r="Y22" t="str">
@@ -2337,27 +2338,27 @@
         <v>21</v>
       </c>
       <c r="B23" t="str">
-        <f>CONCATENATE(A23,"Animation")</f>
+        <f t="shared" si="6"/>
         <v>SOFTWARE_EngineerAnimation</v>
       </c>
-      <c r="C23" s="16">
+      <c r="C23" s="12">
         <f>Timeline!B93</f>
         <v>0.6216216216216216</v>
       </c>
-      <c r="D23" s="16">
+      <c r="D23" s="12">
         <f>Timeline!B129</f>
         <v>0.86486486486486491</v>
       </c>
-      <c r="E23" s="18">
+      <c r="E23" s="14">
         <f t="shared" si="1"/>
         <v>62.162162162162161</v>
       </c>
-      <c r="F23" s="19">
+      <c r="F23" s="15">
         <f t="shared" si="2"/>
         <v>86.486486486486484</v>
       </c>
       <c r="G23" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>@keyframes SOFTWARE_EngineerAnimation { 0%, 62.161% {opacity: 0} 62.162%, 63.513% {opacity: 1} 63.514%, 86.485% {opacity: 0} 86.486%, 87.837% {opacity: 1 } 87.838%, 100% {opacity: 0} }</v>
       </c>
       <c r="Y23" t="str">
@@ -2370,27 +2371,27 @@
         <v>22</v>
       </c>
       <c r="B24" t="str">
-        <f>CONCATENATE(A24,"Animation")</f>
+        <f t="shared" si="6"/>
         <v>SOFTWARE_ENgineer2Animation</v>
       </c>
-      <c r="C24" s="16">
+      <c r="C24" s="12">
         <f>Timeline!B95</f>
         <v>0.63513513513513509</v>
       </c>
-      <c r="D24" s="16">
+      <c r="D24" s="12">
         <f>Timeline!B127</f>
         <v>0.85135135135135132</v>
       </c>
-      <c r="E24" s="18">
+      <c r="E24" s="14">
         <f t="shared" si="1"/>
         <v>63.513513513513509</v>
       </c>
-      <c r="F24" s="19">
+      <c r="F24" s="15">
         <f t="shared" si="2"/>
         <v>85.13513513513513</v>
       </c>
       <c r="G24" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>@keyframes SOFTWARE_ENgineer2Animation { 0%, 63.513% {opacity: 0} 63.514%, 64.864% {opacity: 1} 64.865%, 85.134% {opacity: 0} 85.135%, 86.485% {opacity: 1 } 86.486%, 100% {opacity: 0} }</v>
       </c>
       <c r="Y24" t="str">
@@ -2403,27 +2404,27 @@
         <v>23</v>
       </c>
       <c r="B25" t="str">
-        <f>CONCATENATE(A25,"Animation")</f>
+        <f t="shared" si="6"/>
         <v>SOFTWARE_ENGineer3Animation</v>
       </c>
-      <c r="C25" s="16">
+      <c r="C25" s="12">
         <f>Timeline!B97</f>
         <v>0.64864864864864868</v>
       </c>
-      <c r="D25" s="16">
+      <c r="D25" s="12">
         <f>Timeline!B125</f>
         <v>0.83783783783783783</v>
       </c>
-      <c r="E25" s="18">
+      <c r="E25" s="14">
         <f t="shared" si="1"/>
         <v>64.86486486486487</v>
       </c>
-      <c r="F25" s="19">
+      <c r="F25" s="15">
         <f t="shared" si="2"/>
         <v>83.78378378378379</v>
       </c>
       <c r="G25" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>@keyframes SOFTWARE_ENGineer3Animation { 0%, 64.864% {opacity: 0} 64.865%, 66.215% {opacity: 1} 66.216%, 83.783% {opacity: 0} 83.784%, 85.134% {opacity: 1 } 85.135%, 100% {opacity: 0} }</v>
       </c>
       <c r="Y25" t="str">
@@ -2436,27 +2437,27 @@
         <v>24</v>
       </c>
       <c r="B26" t="str">
-        <f>CONCATENATE(A26,"Animation")</f>
+        <f t="shared" si="6"/>
         <v>SOFTWARE_ENGIneer4Animation</v>
       </c>
-      <c r="C26" s="16">
+      <c r="C26" s="12">
         <f>Timeline!B99</f>
         <v>0.66216216216216217</v>
       </c>
-      <c r="D26" s="16">
+      <c r="D26" s="12">
         <f>Timeline!B123</f>
         <v>0.82432432432432434</v>
       </c>
-      <c r="E26" s="18">
+      <c r="E26" s="14">
         <f t="shared" si="1"/>
         <v>66.21621621621621</v>
       </c>
-      <c r="F26" s="19">
+      <c r="F26" s="15">
         <f t="shared" si="2"/>
         <v>82.432432432432435</v>
       </c>
       <c r="G26" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>@keyframes SOFTWARE_ENGIneer4Animation { 0%, 66.215% {opacity: 0} 66.216%, 67.567% {opacity: 1} 67.568%, 82.431% {opacity: 0} 82.432%, 83.783% {opacity: 1 } 83.784%, 100% {opacity: 0} }</v>
       </c>
       <c r="Y26" t="str">
@@ -2469,27 +2470,27 @@
         <v>25</v>
       </c>
       <c r="B27" t="str">
-        <f>CONCATENATE(A27,"Animation")</f>
+        <f t="shared" si="6"/>
         <v>SOFTWARE_ENGINeer5Animation</v>
       </c>
-      <c r="C27" s="16">
+      <c r="C27" s="12">
         <f>Timeline!B101</f>
         <v>0.67567567567567566</v>
       </c>
-      <c r="D27" s="16">
+      <c r="D27" s="12">
         <f>Timeline!B121</f>
         <v>0.81081081081081086</v>
       </c>
-      <c r="E27" s="18">
+      <c r="E27" s="14">
         <f t="shared" si="1"/>
         <v>67.567567567567565</v>
       </c>
-      <c r="F27" s="19">
+      <c r="F27" s="15">
         <f t="shared" si="2"/>
         <v>81.081081081081081</v>
       </c>
       <c r="G27" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>@keyframes SOFTWARE_ENGINeer5Animation { 0%, 67.567% {opacity: 0} 67.568%, 68.918% {opacity: 1} 68.919%, 81.08% {opacity: 0} 81.081%, 82.431% {opacity: 1 } 82.432%, 100% {opacity: 0} }</v>
       </c>
       <c r="Y27" t="str">
@@ -2502,27 +2503,27 @@
         <v>26</v>
       </c>
       <c r="B28" t="str">
-        <f>CONCATENATE(A28,"Animation")</f>
+        <f t="shared" si="6"/>
         <v>SOFTWARE_ENGINEer6Animation</v>
       </c>
-      <c r="C28" s="16">
+      <c r="C28" s="12">
         <f>Timeline!B103</f>
         <v>0.68918918918918914</v>
       </c>
-      <c r="D28" s="16">
+      <c r="D28" s="12">
         <f>Timeline!B119</f>
         <v>0.79729729729729726</v>
       </c>
-      <c r="E28" s="18">
+      <c r="E28" s="14">
         <f t="shared" si="1"/>
         <v>68.918918918918919</v>
       </c>
-      <c r="F28" s="19">
+      <c r="F28" s="15">
         <f t="shared" si="2"/>
         <v>79.729729729729726</v>
       </c>
       <c r="G28" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>@keyframes SOFTWARE_ENGINEer6Animation { 0%, 68.918% {opacity: 0} 68.919%, 70.269% {opacity: 1} 70.27%, 79.729% {opacity: 0} 79.73%, 81.08% {opacity: 1 } 81.081%, 100% {opacity: 0} }</v>
       </c>
       <c r="Y28" t="str">
@@ -2535,27 +2536,27 @@
         <v>27</v>
       </c>
       <c r="B29" t="str">
-        <f>CONCATENATE(A29,"Animation")</f>
+        <f t="shared" si="6"/>
         <v>SOFTWARE_ENGINEEr7Animation</v>
       </c>
-      <c r="C29" s="16">
+      <c r="C29" s="12">
         <f>Timeline!B105</f>
         <v>0.70270270270270274</v>
       </c>
-      <c r="D29" s="16">
+      <c r="D29" s="12">
         <f>Timeline!B117</f>
         <v>0.78378378378378377</v>
       </c>
-      <c r="E29" s="18">
+      <c r="E29" s="14">
         <f t="shared" si="1"/>
         <v>70.270270270270274</v>
       </c>
-      <c r="F29" s="19">
+      <c r="F29" s="15">
         <f t="shared" si="2"/>
         <v>78.378378378378372</v>
       </c>
       <c r="G29" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>@keyframes SOFTWARE_ENGINEEr7Animation { 0%, 70.269% {opacity: 0} 70.27%, 71.621% {opacity: 1} 71.622%, 78.377% {opacity: 0} 78.378%, 79.729% {opacity: 1 } 79.73%, 100% {opacity: 0} }</v>
       </c>
       <c r="Y29" t="str">
@@ -2568,22 +2569,22 @@
         <v>28</v>
       </c>
       <c r="B30" t="str">
-        <f>CONCATENATE(A30,"Animation")</f>
+        <f t="shared" si="6"/>
         <v>SOFTWARE_ENGINEER8Animation</v>
       </c>
-      <c r="C30" s="16">
+      <c r="C30" s="12">
         <f>Timeline!B107</f>
         <v>0.71621621621621623</v>
       </c>
-      <c r="D30" s="16">
+      <c r="D30" s="12">
         <f>Timeline!B117</f>
         <v>0.78378378378378377</v>
       </c>
-      <c r="E30" s="18">
+      <c r="E30" s="14">
         <f t="shared" si="1"/>
         <v>71.621621621621628</v>
       </c>
-      <c r="F30" s="20">
+      <c r="F30" s="16">
         <f t="shared" si="2"/>
         <v>78.378378378378372</v>
       </c>
@@ -2602,38 +2603,1050 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{248B7C34-87E5-4454-9B14-67B703053C1F}">
+  <dimension ref="A1:Y30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="Y1" sqref="Y1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.6640625" customWidth="1"/>
+    <col min="2" max="4" width="30.5546875" customWidth="1"/>
+    <col min="5" max="5" width="30.5546875" style="12" customWidth="1"/>
+    <col min="6" max="6" width="29.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="str">
+        <f>CONCATENATE(A1,"Animation")</f>
+        <v>FirstLineAnimation</v>
+      </c>
+      <c r="C1" s="12">
+        <f>Timeline!B9</f>
+        <v>5.4054054054054057E-2</v>
+      </c>
+      <c r="D1" s="12">
+        <f>Timeline!B65</f>
+        <v>0.43243243243243246</v>
+      </c>
+      <c r="E1" s="14">
+        <f>C1*100</f>
+        <v>5.4054054054054053</v>
+      </c>
+      <c r="F1" s="16">
+        <f>D1*100</f>
+        <v>43.243243243243242</v>
+      </c>
+      <c r="G1" t="str">
+        <f>CONCATENATE("@keyframes ",B1, " { 0%, 100% {opacity: 1 } }")</f>
+        <v>@keyframes FirstLineAnimation { 0%, 100% {opacity: 1 } }</v>
+      </c>
+      <c r="Y1" t="str">
+        <f>CONCATENATE(".",B1, " { animation: ", B1, " 5.5s linear 1 normal; animation-fill-mode: forwards; }")</f>
+        <v>.FirstLineAnimation { animation: FirstLineAnimation 5.5s linear 1 normal; animation-fill-mode: forwards; }</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="str">
+        <f t="shared" ref="B2:B30" si="0">CONCATENATE(A2,"Animation")</f>
+        <v>CarolineAnimation</v>
+      </c>
+      <c r="C2" s="12">
+        <f>Timeline!B11</f>
+        <v>6.7567567567567571E-2</v>
+      </c>
+      <c r="D2" s="12">
+        <f>Timeline!B63</f>
+        <v>0.41891891891891891</v>
+      </c>
+      <c r="E2" s="14">
+        <f t="shared" ref="E2:F30" si="1">C2*100</f>
+        <v>6.756756756756757</v>
+      </c>
+      <c r="F2" s="16">
+        <f t="shared" si="1"/>
+        <v>41.891891891891895</v>
+      </c>
+      <c r="G2" t="str">
+        <f t="shared" ref="G2:G12" si="2">CONCATENATE("@keyframes ",B2, " { 0%, ",ROUND(E2,3)- 0.001, "% {opacity: 0} ",ROUND(E2,3), "%, ",ROUND(E3,3)-0.001, "% {opacity: 1} ", ROUND(E3,3), "%, ", ROUND(F2, 3)-0.001,"% {opacity: 0} ", ROUND(F2, 3),"%, ", ROUND(F1, 3)-0.001,"% {opacity: 1 } ", ROUND(F1, 3), "%, 100% {opacity: 0} }")</f>
+        <v>@keyframes CarolineAnimation { 0%, 6.756% {opacity: 0} 6.757%, 8.107% {opacity: 1} 8.108%, 41.891% {opacity: 0} 41.892%, 43.242% {opacity: 1 } 43.243%, 100% {opacity: 0} }</v>
+      </c>
+      <c r="H2" s="9"/>
+      <c r="Y2" t="str">
+        <f t="shared" ref="Y2:Y30" si="3">CONCATENATE(".",B2, " { animation: ", B2, " 5.5s linear 1 normal; animation-fill-mode: forwards; }")</f>
+        <v>.CarolineAnimation { animation: CarolineAnimation 5.5s linear 1 normal; animation-fill-mode: forwards; }</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" si="0"/>
+        <v>CAroline2Animation</v>
+      </c>
+      <c r="C3" s="12">
+        <f>Timeline!B13</f>
+        <v>8.1081081081081086E-2</v>
+      </c>
+      <c r="D3" s="12">
+        <f>Timeline!B61</f>
+        <v>0.40540540540540543</v>
+      </c>
+      <c r="E3" s="14">
+        <f t="shared" si="1"/>
+        <v>8.1081081081081088</v>
+      </c>
+      <c r="F3" s="15">
+        <f t="shared" si="1"/>
+        <v>40.54054054054054</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" si="2"/>
+        <v>@keyframes CAroline2Animation { 0%, 8.107% {opacity: 0} 8.108%, 9.458% {opacity: 1} 9.459%, 40.54% {opacity: 0} 40.541%, 41.891% {opacity: 1 } 41.892%, 100% {opacity: 0} }</v>
+      </c>
+      <c r="Y3" t="str">
+        <f t="shared" si="3"/>
+        <v>.CAroline2Animation { animation: CAroline2Animation 5.5s linear 1 normal; animation-fill-mode: forwards; }</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>CARoline3Animation</v>
+      </c>
+      <c r="C4" s="12">
+        <f>Timeline!B15</f>
+        <v>9.45945945945946E-2</v>
+      </c>
+      <c r="D4" s="12">
+        <f>Timeline!B59</f>
+        <v>0.39189189189189189</v>
+      </c>
+      <c r="E4" s="14">
+        <f t="shared" si="1"/>
+        <v>9.4594594594594597</v>
+      </c>
+      <c r="F4" s="15">
+        <f t="shared" si="1"/>
+        <v>39.189189189189186</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="2"/>
+        <v>@keyframes CARoline3Animation { 0%, 9.458% {opacity: 0} 9.459%, 10.81% {opacity: 1} 10.811%, 39.188% {opacity: 0} 39.189%, 40.54% {opacity: 1 } 40.541%, 100% {opacity: 0} }</v>
+      </c>
+      <c r="Y4" t="str">
+        <f t="shared" si="3"/>
+        <v>.CARoline3Animation { animation: CARoline3Animation 5.5s linear 1 normal; animation-fill-mode: forwards; }</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>CAROline4Animation</v>
+      </c>
+      <c r="C5" s="12">
+        <f>Timeline!B17</f>
+        <v>0.10810810810810811</v>
+      </c>
+      <c r="D5" s="12">
+        <f>Timeline!B57</f>
+        <v>0.3783783783783784</v>
+      </c>
+      <c r="E5" s="14">
+        <f t="shared" si="1"/>
+        <v>10.810810810810811</v>
+      </c>
+      <c r="F5" s="15">
+        <f t="shared" si="1"/>
+        <v>37.837837837837839</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="2"/>
+        <v>@keyframes CAROline4Animation { 0%, 10.81% {opacity: 0} 10.811%, 12.161% {opacity: 1} 12.162%, 37.837% {opacity: 0} 37.838%, 39.188% {opacity: 1 } 39.189%, 100% {opacity: 0} }</v>
+      </c>
+      <c r="Y5" t="str">
+        <f t="shared" si="3"/>
+        <v>.CAROline4Animation { animation: CAROline4Animation 5.5s linear 1 normal; animation-fill-mode: forwards; }</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>CAROLine5Animation</v>
+      </c>
+      <c r="C6" s="12">
+        <f>Timeline!B19</f>
+        <v>0.12162162162162163</v>
+      </c>
+      <c r="D6" s="12">
+        <f>Timeline!B55</f>
+        <v>0.36486486486486486</v>
+      </c>
+      <c r="E6" s="14">
+        <f t="shared" si="1"/>
+        <v>12.162162162162163</v>
+      </c>
+      <c r="F6" s="15">
+        <f t="shared" si="1"/>
+        <v>36.486486486486484</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="2"/>
+        <v>@keyframes CAROLine5Animation { 0%, 12.161% {opacity: 0} 12.162%, 13.513% {opacity: 1} 13.514%, 36.485% {opacity: 0} 36.486%, 37.837% {opacity: 1 } 37.838%, 100% {opacity: 0} }</v>
+      </c>
+      <c r="Y6" t="str">
+        <f t="shared" si="3"/>
+        <v>.CAROLine5Animation { animation: CAROLine5Animation 5.5s linear 1 normal; animation-fill-mode: forwards; }</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>CAROLIne6Animation</v>
+      </c>
+      <c r="C7" s="12">
+        <f>Timeline!B21</f>
+        <v>0.13513513513513514</v>
+      </c>
+      <c r="D7" s="12">
+        <f>Timeline!B53</f>
+        <v>0.35135135135135137</v>
+      </c>
+      <c r="E7" s="14">
+        <f t="shared" si="1"/>
+        <v>13.513513513513514</v>
+      </c>
+      <c r="F7" s="15">
+        <f t="shared" si="1"/>
+        <v>35.135135135135137</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="2"/>
+        <v>@keyframes CAROLIne6Animation { 0%, 13.513% {opacity: 0} 13.514%, 14.864% {opacity: 1} 14.865%, 35.134% {opacity: 0} 35.135%, 36.485% {opacity: 1 } 36.486%, 100% {opacity: 0} }</v>
+      </c>
+      <c r="Y7" t="str">
+        <f t="shared" si="3"/>
+        <v>.CAROLIne6Animation { animation: CAROLIne6Animation 5.5s linear 1 normal; animation-fill-mode: forwards; }</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>CAROLINe7Animation</v>
+      </c>
+      <c r="C8" s="12">
+        <f>Timeline!B23</f>
+        <v>0.14864864864864866</v>
+      </c>
+      <c r="D8" s="12">
+        <f>Timeline!B51</f>
+        <v>0.33783783783783783</v>
+      </c>
+      <c r="E8" s="14">
+        <f t="shared" si="1"/>
+        <v>14.864864864864865</v>
+      </c>
+      <c r="F8" s="15">
+        <f t="shared" si="1"/>
+        <v>33.783783783783782</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="2"/>
+        <v>@keyframes CAROLINe7Animation { 0%, 14.864% {opacity: 0} 14.865%, 16.215% {opacity: 1} 16.216%, 33.783% {opacity: 0} 33.784%, 35.134% {opacity: 1 } 35.135%, 100% {opacity: 0} }</v>
+      </c>
+      <c r="Y8" t="str">
+        <f t="shared" si="3"/>
+        <v>.CAROLINe7Animation { animation: CAROLINe7Animation 5.5s linear 1 normal; animation-fill-mode: forwards; }</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>CAROLINE8Animation</v>
+      </c>
+      <c r="C9" s="12">
+        <f>Timeline!B25</f>
+        <v>0.16216216216216217</v>
+      </c>
+      <c r="D9" s="12">
+        <f>Timeline!B49</f>
+        <v>0.32432432432432434</v>
+      </c>
+      <c r="E9" s="14">
+        <f t="shared" si="1"/>
+        <v>16.216216216216218</v>
+      </c>
+      <c r="F9" s="15">
+        <f t="shared" si="1"/>
+        <v>32.432432432432435</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="2"/>
+        <v>@keyframes CAROLINE8Animation { 0%, 16.215% {opacity: 0} 16.216%, 17.567% {opacity: 1} 17.568%, 32.431% {opacity: 0} 32.432%, 33.783% {opacity: 1 } 33.784%, 100% {opacity: 0} }</v>
+      </c>
+      <c r="Y9" t="str">
+        <f t="shared" si="3"/>
+        <v>.CAROLINE8Animation { animation: CAROLINE8Animation 5.5s linear 1 normal; animation-fill-mode: forwards; }</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>CAROLINE_SpaceAnimation</v>
+      </c>
+      <c r="C10" s="12">
+        <f>Timeline!B27</f>
+        <v>0.17567567567567569</v>
+      </c>
+      <c r="D10" s="12">
+        <f>Timeline!B47</f>
+        <v>0.3108108108108108</v>
+      </c>
+      <c r="E10" s="14">
+        <f t="shared" si="1"/>
+        <v>17.567567567567568</v>
+      </c>
+      <c r="F10" s="15">
+        <f t="shared" si="1"/>
+        <v>31.081081081081081</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="2"/>
+        <v>@keyframes CAROLINE_SpaceAnimation { 0%, 17.567% {opacity: 0} 17.568%, 18.918% {opacity: 1} 18.919%, 31.08% {opacity: 0} 31.081%, 32.431% {opacity: 1 } 32.432%, 100% {opacity: 0} }</v>
+      </c>
+      <c r="Y10" t="str">
+        <f t="shared" si="3"/>
+        <v>.CAROLINE_SpaceAnimation { animation: CAROLINE_SpaceAnimation 5.5s linear 1 normal; animation-fill-mode: forwards; }</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>CAROLINE_HamAnimation</v>
+      </c>
+      <c r="C11" s="12">
+        <f>Timeline!B29</f>
+        <v>0.1891891891891892</v>
+      </c>
+      <c r="D11" s="12">
+        <f>Timeline!B45</f>
+        <v>0.29729729729729731</v>
+      </c>
+      <c r="E11" s="14">
+        <f t="shared" si="1"/>
+        <v>18.918918918918919</v>
+      </c>
+      <c r="F11" s="15">
+        <f t="shared" si="1"/>
+        <v>29.72972972972973</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="2"/>
+        <v>@keyframes CAROLINE_HamAnimation { 0%, 18.918% {opacity: 0} 18.919%, 20.269% {opacity: 1} 20.27%, 29.729% {opacity: 0} 29.73%, 31.08% {opacity: 1 } 31.081%, 100% {opacity: 0} }</v>
+      </c>
+      <c r="Y11" t="str">
+        <f t="shared" si="3"/>
+        <v>.CAROLINE_HamAnimation { animation: CAROLINE_HamAnimation 5.5s linear 1 normal; animation-fill-mode: forwards; }</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>CAROLINE_HAm2Animation</v>
+      </c>
+      <c r="C12" s="12">
+        <f>Timeline!B31</f>
+        <v>0.20270270270270271</v>
+      </c>
+      <c r="D12" s="12">
+        <f>Timeline!B43</f>
+        <v>0.28378378378378377</v>
+      </c>
+      <c r="E12" s="14">
+        <f t="shared" si="1"/>
+        <v>20.27027027027027</v>
+      </c>
+      <c r="F12" s="15">
+        <f t="shared" si="1"/>
+        <v>28.378378378378379</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="2"/>
+        <v>@keyframes CAROLINE_HAm2Animation { 0%, 20.269% {opacity: 0} 20.27%, 21.621% {opacity: 1} 21.622%, 28.377% {opacity: 0} 28.378%, 29.729% {opacity: 1 } 29.73%, 100% {opacity: 0} }</v>
+      </c>
+      <c r="Y12" t="str">
+        <f t="shared" si="3"/>
+        <v>.CAROLINE_HAm2Animation { animation: CAROLINE_HAm2Animation 5.5s linear 1 normal; animation-fill-mode: forwards; }</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>CAROLINE_HAM3Animation</v>
+      </c>
+      <c r="C13" s="12">
+        <f>Timeline!B33</f>
+        <v>0.21621621621621623</v>
+      </c>
+      <c r="D13" s="12">
+        <f>Timeline!B43</f>
+        <v>0.28378378378378377</v>
+      </c>
+      <c r="E13" s="14">
+        <f t="shared" si="1"/>
+        <v>21.621621621621621</v>
+      </c>
+      <c r="F13" s="16">
+        <f t="shared" si="1"/>
+        <v>28.378378378378379</v>
+      </c>
+      <c r="G13" t="str">
+        <f>CONCATENATE("@keyframes ",B13, " { 0%, ",ROUND(E13,3)- 0.001, "% {opacity: 0} ",ROUND(E13,3), "%, ", ROUND(F13, 3)-0.001,"% {opacity: 1} ", ROUND(F13, 3),"%, 100% {opacity: 0} }")</f>
+        <v>@keyframes CAROLINE_HAM3Animation { 0%, 21.621% {opacity: 0} 21.622%, 28.377% {opacity: 1} 28.378%, 100% {opacity: 0} }</v>
+      </c>
+      <c r="Y13" t="str">
+        <f t="shared" si="3"/>
+        <v>.CAROLINE_HAM3Animation { animation: CAROLINE_HAM3Animation 5.5s linear 1 normal; animation-fill-mode: forwards; }</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>SoftwareAnimation</v>
+      </c>
+      <c r="C14" s="12">
+        <f>Timeline!B75</f>
+        <v>0.5</v>
+      </c>
+      <c r="D14" s="12">
+        <f>Timeline!B147</f>
+        <v>0.98648648648648651</v>
+      </c>
+      <c r="E14" s="14">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="F14" s="16">
+        <f t="shared" si="1"/>
+        <v>98.648648648648646</v>
+      </c>
+      <c r="G14" t="str">
+        <f>CONCATENATE("@keyframes ",B14, " { 0%, ",ROUND(E14,3)- 0.001, "% {opacity: 0} ",ROUND(E14,3), "%, ",ROUND(E15,3)-0.001, "% {opacity: 1} ", ROUND(E15,3), "%, ", ROUND(F14, 3)-0.001,"% {opacity: 0} ", ROUND(F14, 3),"%, 99.98% {opacity: 1} 99.99%, 100% {opacity: 0} }")</f>
+        <v>@keyframes SoftwareAnimation { 0%, 49.999% {opacity: 0} 50%, 51.35% {opacity: 1} 51.351%, 98.648% {opacity: 0} 98.649%, 99.98% {opacity: 1} 99.99%, 100% {opacity: 0} }</v>
+      </c>
+      <c r="Y14" t="str">
+        <f t="shared" si="3"/>
+        <v>.SoftwareAnimation { animation: SoftwareAnimation 5.5s linear 1 normal; animation-fill-mode: forwards; }</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>SOftware2Animation</v>
+      </c>
+      <c r="C15" s="12">
+        <f>Timeline!B77</f>
+        <v>0.51351351351351349</v>
+      </c>
+      <c r="D15" s="12">
+        <f>Timeline!B145</f>
+        <v>0.97297297297297303</v>
+      </c>
+      <c r="E15" s="14">
+        <f t="shared" si="1"/>
+        <v>51.351351351351347</v>
+      </c>
+      <c r="F15" s="17">
+        <f t="shared" si="1"/>
+        <v>97.297297297297305</v>
+      </c>
+      <c r="G15" t="str">
+        <f>CONCATENATE("@keyframes ",B15, " { 0%, ",ROUND(E15,3)- 0.001, "% {opacity: 0} ",ROUND(E15,3), "%, ",ROUND(E16,3)-0.001, "% {opacity: 1} ", ROUND(E16,3), "%, ", ROUND(F15, 3)-0.001,"% {opacity: 0} ", ROUND(F15, 3),"%, ", ROUND(F14, 3)-0.001,"% {opacity: 1 } ", ROUND(F14, 3), "%, 100% {opacity: 0} }")</f>
+        <v>@keyframes SOftware2Animation { 0%, 51.35% {opacity: 0} 51.351%, 52.702% {opacity: 1} 52.703%, 97.296% {opacity: 0} 97.297%, 98.648% {opacity: 1 } 98.649%, 100% {opacity: 0} }</v>
+      </c>
+      <c r="Y15" t="str">
+        <f t="shared" si="3"/>
+        <v>.SOftware2Animation { animation: SOftware2Animation 5.5s linear 1 normal; animation-fill-mode: forwards; }</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>SOFtware3Animation</v>
+      </c>
+      <c r="C16" s="12">
+        <f>Timeline!B79</f>
+        <v>0.52702702702702697</v>
+      </c>
+      <c r="D16" s="12">
+        <f>Timeline!B143</f>
+        <v>0.95945945945945943</v>
+      </c>
+      <c r="E16" s="14">
+        <f t="shared" si="1"/>
+        <v>52.702702702702695</v>
+      </c>
+      <c r="F16" s="15">
+        <f t="shared" si="1"/>
+        <v>95.945945945945937</v>
+      </c>
+      <c r="G16" t="str">
+        <f>CONCATENATE("@keyframes ",B16, " { 0%, ",ROUND(E16,3)- 0.001, "% {opacity: 0} ",ROUND(E16,3), "%, ",ROUND(E17,3)-0.001, "% {opacity: 1} ", ROUND(E17,3), "%, ", ROUND(F16, 3)-0.001,"% {opacity: 0} ", ROUND(F16, 3),"%, ", ROUND(F15, 3)-0.001,"% {opacity: 1 } ", ROUND(F15, 3), "%, 100% {opacity: 0} }")</f>
+        <v>@keyframes SOFtware3Animation { 0%, 52.702% {opacity: 0} 52.703%, 54.053% {opacity: 1} 54.054%, 95.945% {opacity: 0} 95.946%, 97.296% {opacity: 1 } 97.297%, 100% {opacity: 0} }</v>
+      </c>
+      <c r="Y16" t="str">
+        <f t="shared" si="3"/>
+        <v>.SOFtware3Animation { animation: SOFtware3Animation 5.5s linear 1 normal; animation-fill-mode: forwards; }</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>SOFTware4Animation</v>
+      </c>
+      <c r="C17" s="12">
+        <f>Timeline!B81</f>
+        <v>0.54054054054054057</v>
+      </c>
+      <c r="D17" s="12">
+        <f>Timeline!B141</f>
+        <v>0.94594594594594594</v>
+      </c>
+      <c r="E17" s="14">
+        <f t="shared" si="1"/>
+        <v>54.054054054054056</v>
+      </c>
+      <c r="F17" s="15">
+        <f t="shared" si="1"/>
+        <v>94.594594594594597</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" ref="G17:G29" si="4">CONCATENATE("@keyframes ",B17, " { 0%, ",ROUND(E17,3)- 0.001, "% {opacity: 0} ",ROUND(E17,3), "%, ",ROUND(E18,3)-0.001, "% {opacity: 1} ", ROUND(E18,3), "%, ", ROUND(F17, 3)-0.001,"% {opacity: 0} ", ROUND(F17, 3),"%, ", ROUND(F16, 3)-0.001,"% {opacity: 1 } ", ROUND(F16, 3), "%, 100% {opacity: 0} }")</f>
+        <v>@keyframes SOFTware4Animation { 0%, 54.053% {opacity: 0} 54.054%, 55.404% {opacity: 1} 55.405%, 94.594% {opacity: 0} 94.595%, 95.945% {opacity: 1 } 95.946%, 100% {opacity: 0} }</v>
+      </c>
+      <c r="Y17" t="str">
+        <f t="shared" si="3"/>
+        <v>.SOFTware4Animation { animation: SOFTware4Animation 5.5s linear 1 normal; animation-fill-mode: forwards; }</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" t="str">
+        <f t="shared" si="0"/>
+        <v>SOFTWare5Animation</v>
+      </c>
+      <c r="C18" s="12">
+        <f>Timeline!B83</f>
+        <v>0.55405405405405406</v>
+      </c>
+      <c r="D18" s="12">
+        <f>Timeline!B139</f>
+        <v>0.93243243243243246</v>
+      </c>
+      <c r="E18" s="14">
+        <f t="shared" si="1"/>
+        <v>55.405405405405403</v>
+      </c>
+      <c r="F18" s="15">
+        <f t="shared" si="1"/>
+        <v>93.243243243243242</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="4"/>
+        <v>@keyframes SOFTWare5Animation { 0%, 55.404% {opacity: 0} 55.405%, 56.756% {opacity: 1} 56.757%, 93.242% {opacity: 0} 93.243%, 94.594% {opacity: 1 } 94.595%, 100% {opacity: 0} }</v>
+      </c>
+      <c r="Y18" t="str">
+        <f t="shared" si="3"/>
+        <v>.SOFTWare5Animation { animation: SOFTWare5Animation 5.5s linear 1 normal; animation-fill-mode: forwards; }</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" t="str">
+        <f t="shared" si="0"/>
+        <v>SOFTWAre6Animation</v>
+      </c>
+      <c r="C19" s="12">
+        <f>Timeline!B85</f>
+        <v>0.56756756756756754</v>
+      </c>
+      <c r="D19" s="12">
+        <f>Timeline!B137</f>
+        <v>0.91891891891891897</v>
+      </c>
+      <c r="E19" s="14">
+        <f t="shared" si="1"/>
+        <v>56.756756756756758</v>
+      </c>
+      <c r="F19" s="15">
+        <f t="shared" si="1"/>
+        <v>91.891891891891902</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="4"/>
+        <v>@keyframes SOFTWAre6Animation { 0%, 56.756% {opacity: 0} 56.757%, 58.107% {opacity: 1} 58.108%, 91.891% {opacity: 0} 91.892%, 93.242% {opacity: 1 } 93.243%, 100% {opacity: 0} }</v>
+      </c>
+      <c r="Y19" t="str">
+        <f t="shared" si="3"/>
+        <v>.SOFTWAre6Animation { animation: SOFTWAre6Animation 5.5s linear 1 normal; animation-fill-mode: forwards; }</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" t="str">
+        <f t="shared" si="0"/>
+        <v>SOFTWARe7Animation</v>
+      </c>
+      <c r="C20" s="12">
+        <f>Timeline!B87</f>
+        <v>0.58108108108108103</v>
+      </c>
+      <c r="D20" s="12">
+        <f>Timeline!B135</f>
+        <v>0.90540540540540537</v>
+      </c>
+      <c r="E20" s="14">
+        <f t="shared" si="1"/>
+        <v>58.108108108108105</v>
+      </c>
+      <c r="F20" s="15">
+        <f t="shared" si="1"/>
+        <v>90.540540540540533</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="4"/>
+        <v>@keyframes SOFTWARe7Animation { 0%, 58.107% {opacity: 0} 58.108%, 59.458% {opacity: 1} 59.459%, 90.54% {opacity: 0} 90.541%, 91.891% {opacity: 1 } 91.892%, 100% {opacity: 0} }</v>
+      </c>
+      <c r="Y20" t="str">
+        <f t="shared" si="3"/>
+        <v>.SOFTWARe7Animation { animation: SOFTWARe7Animation 5.5s linear 1 normal; animation-fill-mode: forwards; }</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" t="str">
+        <f t="shared" si="0"/>
+        <v>SOFTWARE8Animation</v>
+      </c>
+      <c r="C21" s="12">
+        <f>Timeline!B89</f>
+        <v>0.59459459459459463</v>
+      </c>
+      <c r="D21" s="12">
+        <f>Timeline!B133</f>
+        <v>0.89189189189189189</v>
+      </c>
+      <c r="E21" s="14">
+        <f t="shared" si="1"/>
+        <v>59.45945945945946</v>
+      </c>
+      <c r="F21" s="15">
+        <f t="shared" si="1"/>
+        <v>89.189189189189193</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="4"/>
+        <v>@keyframes SOFTWARE8Animation { 0%, 59.458% {opacity: 0} 59.459%, 60.81% {opacity: 1} 60.811%, 89.188% {opacity: 0} 89.189%, 90.54% {opacity: 1 } 90.541%, 100% {opacity: 0} }</v>
+      </c>
+      <c r="Y21" t="str">
+        <f t="shared" si="3"/>
+        <v>.SOFTWARE8Animation { animation: SOFTWARE8Animation 5.5s linear 1 normal; animation-fill-mode: forwards; }</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" t="str">
+        <f t="shared" si="0"/>
+        <v>SOFTWARE_SpaceAnimation</v>
+      </c>
+      <c r="C22" s="12">
+        <f>Timeline!B91</f>
+        <v>0.60810810810810811</v>
+      </c>
+      <c r="D22" s="12">
+        <f>Timeline!B131</f>
+        <v>0.8783783783783784</v>
+      </c>
+      <c r="E22" s="14">
+        <f t="shared" si="1"/>
+        <v>60.810810810810814</v>
+      </c>
+      <c r="F22" s="15">
+        <f t="shared" si="1"/>
+        <v>87.837837837837839</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="4"/>
+        <v>@keyframes SOFTWARE_SpaceAnimation { 0%, 60.81% {opacity: 0} 60.811%, 62.161% {opacity: 1} 62.162%, 87.837% {opacity: 0} 87.838%, 89.188% {opacity: 1 } 89.189%, 100% {opacity: 0} }</v>
+      </c>
+      <c r="Y22" t="str">
+        <f t="shared" si="3"/>
+        <v>.SOFTWARE_SpaceAnimation { animation: SOFTWARE_SpaceAnimation 5.5s linear 1 normal; animation-fill-mode: forwards; }</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" t="str">
+        <f t="shared" si="0"/>
+        <v>SOFTWARE_EngineerAnimation</v>
+      </c>
+      <c r="C23" s="12">
+        <f>Timeline!B93</f>
+        <v>0.6216216216216216</v>
+      </c>
+      <c r="D23" s="12">
+        <f>Timeline!B129</f>
+        <v>0.86486486486486491</v>
+      </c>
+      <c r="E23" s="14">
+        <f t="shared" si="1"/>
+        <v>62.162162162162161</v>
+      </c>
+      <c r="F23" s="15">
+        <f t="shared" si="1"/>
+        <v>86.486486486486484</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="4"/>
+        <v>@keyframes SOFTWARE_EngineerAnimation { 0%, 62.161% {opacity: 0} 62.162%, 63.513% {opacity: 1} 63.514%, 86.485% {opacity: 0} 86.486%, 87.837% {opacity: 1 } 87.838%, 100% {opacity: 0} }</v>
+      </c>
+      <c r="Y23" t="str">
+        <f t="shared" si="3"/>
+        <v>.SOFTWARE_EngineerAnimation { animation: SOFTWARE_EngineerAnimation 5.5s linear 1 normal; animation-fill-mode: forwards; }</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" t="str">
+        <f t="shared" si="0"/>
+        <v>SOFTWARE_ENgineer2Animation</v>
+      </c>
+      <c r="C24" s="12">
+        <f>Timeline!B95</f>
+        <v>0.63513513513513509</v>
+      </c>
+      <c r="D24" s="12">
+        <f>Timeline!B127</f>
+        <v>0.85135135135135132</v>
+      </c>
+      <c r="E24" s="14">
+        <f t="shared" si="1"/>
+        <v>63.513513513513509</v>
+      </c>
+      <c r="F24" s="15">
+        <f t="shared" si="1"/>
+        <v>85.13513513513513</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="4"/>
+        <v>@keyframes SOFTWARE_ENgineer2Animation { 0%, 63.513% {opacity: 0} 63.514%, 64.864% {opacity: 1} 64.865%, 85.134% {opacity: 0} 85.135%, 86.485% {opacity: 1 } 86.486%, 100% {opacity: 0} }</v>
+      </c>
+      <c r="Y24" t="str">
+        <f t="shared" si="3"/>
+        <v>.SOFTWARE_ENgineer2Animation { animation: SOFTWARE_ENgineer2Animation 5.5s linear 1 normal; animation-fill-mode: forwards; }</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A25" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" t="str">
+        <f t="shared" si="0"/>
+        <v>SOFTWARE_ENGineer3Animation</v>
+      </c>
+      <c r="C25" s="12">
+        <f>Timeline!B97</f>
+        <v>0.64864864864864868</v>
+      </c>
+      <c r="D25" s="12">
+        <f>Timeline!B125</f>
+        <v>0.83783783783783783</v>
+      </c>
+      <c r="E25" s="14">
+        <f t="shared" si="1"/>
+        <v>64.86486486486487</v>
+      </c>
+      <c r="F25" s="15">
+        <f t="shared" si="1"/>
+        <v>83.78378378378379</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="4"/>
+        <v>@keyframes SOFTWARE_ENGineer3Animation { 0%, 64.864% {opacity: 0} 64.865%, 66.215% {opacity: 1} 66.216%, 83.783% {opacity: 0} 83.784%, 85.134% {opacity: 1 } 85.135%, 100% {opacity: 0} }</v>
+      </c>
+      <c r="Y25" t="str">
+        <f t="shared" si="3"/>
+        <v>.SOFTWARE_ENGineer3Animation { animation: SOFTWARE_ENGineer3Animation 5.5s linear 1 normal; animation-fill-mode: forwards; }</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A26" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" t="str">
+        <f t="shared" si="0"/>
+        <v>SOFTWARE_ENGIneer4Animation</v>
+      </c>
+      <c r="C26" s="12">
+        <f>Timeline!B99</f>
+        <v>0.66216216216216217</v>
+      </c>
+      <c r="D26" s="12">
+        <f>Timeline!B123</f>
+        <v>0.82432432432432434</v>
+      </c>
+      <c r="E26" s="14">
+        <f t="shared" si="1"/>
+        <v>66.21621621621621</v>
+      </c>
+      <c r="F26" s="15">
+        <f t="shared" si="1"/>
+        <v>82.432432432432435</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="4"/>
+        <v>@keyframes SOFTWARE_ENGIneer4Animation { 0%, 66.215% {opacity: 0} 66.216%, 67.567% {opacity: 1} 67.568%, 82.431% {opacity: 0} 82.432%, 83.783% {opacity: 1 } 83.784%, 100% {opacity: 0} }</v>
+      </c>
+      <c r="Y26" t="str">
+        <f t="shared" si="3"/>
+        <v>.SOFTWARE_ENGIneer4Animation { animation: SOFTWARE_ENGIneer4Animation 5.5s linear 1 normal; animation-fill-mode: forwards; }</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" t="str">
+        <f t="shared" si="0"/>
+        <v>SOFTWARE_ENGINeer5Animation</v>
+      </c>
+      <c r="C27" s="12">
+        <f>Timeline!B101</f>
+        <v>0.67567567567567566</v>
+      </c>
+      <c r="D27" s="12">
+        <f>Timeline!B121</f>
+        <v>0.81081081081081086</v>
+      </c>
+      <c r="E27" s="14">
+        <f t="shared" si="1"/>
+        <v>67.567567567567565</v>
+      </c>
+      <c r="F27" s="15">
+        <f t="shared" si="1"/>
+        <v>81.081081081081081</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="4"/>
+        <v>@keyframes SOFTWARE_ENGINeer5Animation { 0%, 67.567% {opacity: 0} 67.568%, 68.918% {opacity: 1} 68.919%, 81.08% {opacity: 0} 81.081%, 82.431% {opacity: 1 } 82.432%, 100% {opacity: 0} }</v>
+      </c>
+      <c r="Y27" t="str">
+        <f t="shared" si="3"/>
+        <v>.SOFTWARE_ENGINeer5Animation { animation: SOFTWARE_ENGINeer5Animation 5.5s linear 1 normal; animation-fill-mode: forwards; }</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A28" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" t="str">
+        <f t="shared" si="0"/>
+        <v>SOFTWARE_ENGINEer6Animation</v>
+      </c>
+      <c r="C28" s="12">
+        <f>Timeline!B103</f>
+        <v>0.68918918918918914</v>
+      </c>
+      <c r="D28" s="12">
+        <f>Timeline!B119</f>
+        <v>0.79729729729729726</v>
+      </c>
+      <c r="E28" s="14">
+        <f t="shared" si="1"/>
+        <v>68.918918918918919</v>
+      </c>
+      <c r="F28" s="15">
+        <f t="shared" si="1"/>
+        <v>79.729729729729726</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="4"/>
+        <v>@keyframes SOFTWARE_ENGINEer6Animation { 0%, 68.918% {opacity: 0} 68.919%, 70.269% {opacity: 1} 70.27%, 79.729% {opacity: 0} 79.73%, 81.08% {opacity: 1 } 81.081%, 100% {opacity: 0} }</v>
+      </c>
+      <c r="Y28" t="str">
+        <f t="shared" si="3"/>
+        <v>.SOFTWARE_ENGINEer6Animation { animation: SOFTWARE_ENGINEer6Animation 5.5s linear 1 normal; animation-fill-mode: forwards; }</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A29" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" t="str">
+        <f t="shared" si="0"/>
+        <v>SOFTWARE_ENGINEEr7Animation</v>
+      </c>
+      <c r="C29" s="12">
+        <f>Timeline!B105</f>
+        <v>0.70270270270270274</v>
+      </c>
+      <c r="D29" s="12">
+        <f>Timeline!B117</f>
+        <v>0.78378378378378377</v>
+      </c>
+      <c r="E29" s="14">
+        <f t="shared" si="1"/>
+        <v>70.270270270270274</v>
+      </c>
+      <c r="F29" s="15">
+        <f t="shared" si="1"/>
+        <v>78.378378378378372</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="4"/>
+        <v>@keyframes SOFTWARE_ENGINEEr7Animation { 0%, 70.269% {opacity: 0} 70.27%, 71.621% {opacity: 1} 71.622%, 78.377% {opacity: 0} 78.378%, 79.729% {opacity: 1 } 79.73%, 100% {opacity: 0} }</v>
+      </c>
+      <c r="Y29" t="str">
+        <f t="shared" si="3"/>
+        <v>.SOFTWARE_ENGINEEr7Animation { animation: SOFTWARE_ENGINEEr7Animation 5.5s linear 1 normal; animation-fill-mode: forwards; }</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A30" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" t="str">
+        <f t="shared" si="0"/>
+        <v>SOFTWARE_ENGINEER8Animation</v>
+      </c>
+      <c r="C30" s="12">
+        <f>Timeline!B107</f>
+        <v>0.71621621621621623</v>
+      </c>
+      <c r="D30" s="12">
+        <f>Timeline!B117</f>
+        <v>0.78378378378378377</v>
+      </c>
+      <c r="E30" s="14">
+        <f t="shared" si="1"/>
+        <v>71.621621621621628</v>
+      </c>
+      <c r="F30" s="16">
+        <f t="shared" si="1"/>
+        <v>78.378378378378372</v>
+      </c>
+      <c r="G30" t="str">
+        <f>CONCATENATE("@keyframes ",B30, " { 0%, ",ROUND(E30,3)-0.001, "% {opacity: 0} ",ROUND(E30,3), "%, ",ROUND(F30, 3)-0.001, "% {opacity: 1} ", ROUND(F30, 3),"%, 100% {opacity: 0} }")</f>
+        <v>@keyframes SOFTWARE_ENGINEER8Animation { 0%, 71.621% {opacity: 0} 71.622%, 78.377% {opacity: 1} 78.378%, 100% {opacity: 0} }</v>
+      </c>
+      <c r="Y30" t="str">
+        <f t="shared" si="3"/>
+        <v>.SOFTWARE_ENGINEER8Animation { animation: SOFTWARE_ENGINEER8Animation 5.5s linear 1 normal; animation-fill-mode: forwards; }</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14038906-221E-48C3-A3AE-974B8C8595E1}">
   <dimension ref="A1:AO257"/>
   <sheetViews>
-    <sheetView topLeftCell="A50" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+    <sheetView topLeftCell="A54" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.44140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.88671875" style="15" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.88671875" style="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>0</v>
       </c>
-      <c r="B1" s="16">
+      <c r="B1" s="12">
         <f>IF(NOT(ISBLANK(A1)), A1/9.25, "")</f>
         <v>0</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="19" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
-      <c r="B2" s="16" t="str">
+      <c r="B2" s="12" t="str">
         <f t="shared" ref="B2:B65" si="0">IF(NOT(ISBLANK(A2)), A2/9.25, "")</f>
         <v/>
       </c>
-      <c r="C2" s="10"/>
+      <c r="C2" s="19"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="R2" s="2"/>
@@ -2654,71 +3667,71 @@
       <c r="A3">
         <v>0.125</v>
       </c>
-      <c r="B3" s="16">
+      <c r="B3" s="12">
         <f t="shared" si="0"/>
         <v>1.3513513513513514E-2</v>
       </c>
-      <c r="C3" s="10"/>
+      <c r="C3" s="19"/>
     </row>
     <row r="4" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="B4" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C4" s="10"/>
+      <c r="B4" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C4" s="19"/>
     </row>
     <row r="5" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0.25</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B5" s="12">
         <f t="shared" si="0"/>
         <v>2.7027027027027029E-2</v>
       </c>
-      <c r="C5" s="10"/>
+      <c r="C5" s="19"/>
     </row>
     <row r="6" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
-      <c r="B6" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C6" s="10"/>
+      <c r="B6" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C6" s="19"/>
     </row>
     <row r="7" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>0.375</v>
       </c>
-      <c r="B7" s="16">
+      <c r="B7" s="12">
         <f t="shared" si="0"/>
         <v>4.0540540540540543E-2</v>
       </c>
-      <c r="C7" s="10"/>
+      <c r="C7" s="19"/>
     </row>
     <row r="8" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="B8" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C8" s="10"/>
+      <c r="B8" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C8" s="19"/>
     </row>
     <row r="9" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>0.5</v>
       </c>
-      <c r="B9" s="16">
+      <c r="B9" s="12">
         <f t="shared" si="0"/>
         <v>5.4054054054054057E-2</v>
       </c>
-      <c r="C9" s="11"/>
+      <c r="C9" s="20"/>
     </row>
     <row r="10" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
-      <c r="B10" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C10" s="13" t="s">
+      <c r="B10" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C10" s="21" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2726,18 +3739,18 @@
       <c r="A11">
         <v>0.625</v>
       </c>
-      <c r="B11" s="16">
+      <c r="B11" s="12">
         <f t="shared" si="0"/>
         <v>6.7567567567567571E-2</v>
       </c>
-      <c r="C11" s="14"/>
+      <c r="C11" s="18"/>
     </row>
     <row r="12" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="B12" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C12" s="14" t="s">
+      <c r="B12" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C12" s="18" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2745,19 +3758,19 @@
       <c r="A13">
         <v>0.75</v>
       </c>
-      <c r="B13" s="16">
+      <c r="B13" s="12">
         <f t="shared" si="0"/>
         <v>8.1081081081081086E-2</v>
       </c>
-      <c r="C13" s="14"/>
+      <c r="C13" s="18"/>
     </row>
     <row r="14" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
-      <c r="B14" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C14" s="14" t="s">
+      <c r="B14" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C14" s="18" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2765,18 +3778,18 @@
       <c r="A15">
         <v>0.875</v>
       </c>
-      <c r="B15" s="16">
+      <c r="B15" s="12">
         <f t="shared" si="0"/>
         <v>9.45945945945946E-2</v>
       </c>
-      <c r="C15" s="14"/>
+      <c r="C15" s="18"/>
     </row>
     <row r="16" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="B16" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C16" s="14" t="s">
+      <c r="B16" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C16" s="18" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2784,19 +3797,19 @@
       <c r="A17">
         <v>1</v>
       </c>
-      <c r="B17" s="16">
+      <c r="B17" s="12">
         <f t="shared" si="0"/>
         <v>0.10810810810810811</v>
       </c>
-      <c r="C17" s="14"/>
+      <c r="C17" s="18"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
-      <c r="B18" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C18" s="14" t="s">
+      <c r="B18" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C18" s="18" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2804,18 +3817,18 @@
       <c r="A19">
         <v>1.125</v>
       </c>
-      <c r="B19" s="16">
+      <c r="B19" s="12">
         <f t="shared" si="0"/>
         <v>0.12162162162162163</v>
       </c>
-      <c r="C19" s="14"/>
+      <c r="C19" s="18"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B20" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C20" s="14" t="s">
+      <c r="B20" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C20" s="18" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2823,19 +3836,19 @@
       <c r="A21">
         <v>1.25</v>
       </c>
-      <c r="B21" s="16">
+      <c r="B21" s="12">
         <f t="shared" si="0"/>
         <v>0.13513513513513514</v>
       </c>
-      <c r="C21" s="14"/>
+      <c r="C21" s="18"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
-      <c r="B22" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C22" s="14" t="s">
+      <c r="B22" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C22" s="18" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2843,18 +3856,18 @@
       <c r="A23">
         <v>1.375</v>
       </c>
-      <c r="B23" s="16">
+      <c r="B23" s="12">
         <f t="shared" si="0"/>
         <v>0.14864864864864866</v>
       </c>
-      <c r="C23" s="14"/>
+      <c r="C23" s="18"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B24" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C24" s="14" t="s">
+      <c r="B24" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C24" s="18" t="s">
         <v>42</v>
       </c>
     </row>
@@ -2862,19 +3875,19 @@
       <c r="A25">
         <v>1.5</v>
       </c>
-      <c r="B25" s="16">
+      <c r="B25" s="12">
         <f t="shared" si="0"/>
         <v>0.16216216216216217</v>
       </c>
-      <c r="C25" s="14"/>
+      <c r="C25" s="18"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
-      <c r="B26" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C26" s="14" t="s">
+      <c r="B26" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C26" s="18" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2882,18 +3895,18 @@
       <c r="A27">
         <v>1.625</v>
       </c>
-      <c r="B27" s="16">
+      <c r="B27" s="12">
         <f t="shared" si="0"/>
         <v>0.17567567567567569</v>
       </c>
-      <c r="C27" s="14"/>
+      <c r="C27" s="18"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B28" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C28" s="14" t="s">
+      <c r="B28" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C28" s="18" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2901,19 +3914,19 @@
       <c r="A29">
         <v>1.75</v>
       </c>
-      <c r="B29" s="16">
+      <c r="B29" s="12">
         <f t="shared" si="0"/>
         <v>0.1891891891891892</v>
       </c>
-      <c r="C29" s="14"/>
+      <c r="C29" s="18"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
-      <c r="B30" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C30" s="14" t="s">
+      <c r="B30" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C30" s="18" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2921,18 +3934,18 @@
       <c r="A31">
         <v>1.875</v>
       </c>
-      <c r="B31" s="16">
+      <c r="B31" s="12">
         <f t="shared" si="0"/>
         <v>0.20270270270270271</v>
       </c>
-      <c r="C31" s="14"/>
+      <c r="C31" s="18"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B32" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C32" s="14" t="s">
+      <c r="B32" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C32" s="18" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2940,89 +3953,89 @@
       <c r="A33">
         <v>2</v>
       </c>
-      <c r="B33" s="16">
+      <c r="B33" s="12">
         <f t="shared" si="0"/>
         <v>0.21621621621621623</v>
       </c>
-      <c r="C33" s="14"/>
+      <c r="C33" s="18"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
-      <c r="B34" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C34" s="14"/>
+      <c r="B34" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C34" s="18"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>2.125</v>
       </c>
-      <c r="B35" s="16">
+      <c r="B35" s="12">
         <f t="shared" si="0"/>
         <v>0.22972972972972974</v>
       </c>
-      <c r="C35" s="14"/>
+      <c r="C35" s="18"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B36" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C36" s="14"/>
+      <c r="B36" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C36" s="18"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>2.25</v>
       </c>
-      <c r="B37" s="16">
+      <c r="B37" s="12">
         <f t="shared" si="0"/>
         <v>0.24324324324324326</v>
       </c>
-      <c r="C37" s="14"/>
+      <c r="C37" s="18"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="2"/>
-      <c r="B38" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C38" s="14"/>
+      <c r="B38" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C38" s="18"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>2.375</v>
       </c>
-      <c r="B39" s="16">
+      <c r="B39" s="12">
         <f t="shared" si="0"/>
         <v>0.25675675675675674</v>
       </c>
-      <c r="C39" s="14"/>
+      <c r="C39" s="18"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B40" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C40" s="14"/>
+      <c r="B40" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C40" s="18"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>2.5</v>
       </c>
-      <c r="B41" s="16">
+      <c r="B41" s="12">
         <f t="shared" si="0"/>
         <v>0.27027027027027029</v>
       </c>
-      <c r="C41" s="14"/>
+      <c r="C41" s="18"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="2"/>
-      <c r="B42" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C42" s="14" t="s">
+      <c r="B42" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C42" s="18" t="s">
         <v>36</v>
       </c>
     </row>
@@ -3030,18 +4043,18 @@
       <c r="A43">
         <v>2.625</v>
       </c>
-      <c r="B43" s="16">
+      <c r="B43" s="12">
         <f t="shared" si="0"/>
         <v>0.28378378378378377</v>
       </c>
-      <c r="C43" s="14"/>
+      <c r="C43" s="18"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B44" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C44" s="14" t="s">
+      <c r="B44" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C44" s="18" t="s">
         <v>44</v>
       </c>
     </row>
@@ -3049,19 +4062,19 @@
       <c r="A45">
         <v>2.75</v>
       </c>
-      <c r="B45" s="16">
+      <c r="B45" s="12">
         <f t="shared" si="0"/>
         <v>0.29729729729729731</v>
       </c>
-      <c r="C45" s="14"/>
+      <c r="C45" s="18"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="2"/>
-      <c r="B46" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C46" s="14" t="s">
+      <c r="B46" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C46" s="18" t="s">
         <v>43</v>
       </c>
     </row>
@@ -3069,18 +4082,18 @@
       <c r="A47">
         <v>2.875</v>
       </c>
-      <c r="B47" s="16">
+      <c r="B47" s="12">
         <f t="shared" si="0"/>
         <v>0.3108108108108108</v>
       </c>
-      <c r="C47" s="14"/>
+      <c r="C47" s="18"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B48" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C48" s="14" t="s">
+      <c r="B48" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C48" s="18" t="s">
         <v>42</v>
       </c>
     </row>
@@ -3088,19 +4101,19 @@
       <c r="A49">
         <v>3</v>
       </c>
-      <c r="B49" s="16">
+      <c r="B49" s="12">
         <f t="shared" si="0"/>
         <v>0.32432432432432434</v>
       </c>
-      <c r="C49" s="14"/>
+      <c r="C49" s="18"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="2"/>
-      <c r="B50" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C50" s="14" t="s">
+      <c r="B50" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C50" s="18" t="s">
         <v>41</v>
       </c>
     </row>
@@ -3108,18 +4121,18 @@
       <c r="A51">
         <v>3.125</v>
       </c>
-      <c r="B51" s="16">
+      <c r="B51" s="12">
         <f t="shared" si="0"/>
         <v>0.33783783783783783</v>
       </c>
-      <c r="C51" s="14"/>
+      <c r="C51" s="18"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B52" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C52" s="14" t="s">
+      <c r="B52" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C52" s="18" t="s">
         <v>40</v>
       </c>
     </row>
@@ -3127,19 +4140,19 @@
       <c r="A53">
         <v>3.25</v>
       </c>
-      <c r="B53" s="16">
+      <c r="B53" s="12">
         <f t="shared" si="0"/>
         <v>0.35135135135135137</v>
       </c>
-      <c r="C53" s="14"/>
+      <c r="C53" s="18"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="2"/>
-      <c r="B54" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C54" s="14" t="s">
+      <c r="B54" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C54" s="18" t="s">
         <v>39</v>
       </c>
     </row>
@@ -3147,18 +4160,18 @@
       <c r="A55">
         <v>3.375</v>
       </c>
-      <c r="B55" s="16">
+      <c r="B55" s="12">
         <f t="shared" si="0"/>
         <v>0.36486486486486486</v>
       </c>
-      <c r="C55" s="14"/>
+      <c r="C55" s="18"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B56" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C56" s="14" t="s">
+      <c r="B56" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C56" s="18" t="s">
         <v>38</v>
       </c>
     </row>
@@ -3166,19 +4179,19 @@
       <c r="A57">
         <v>3.5</v>
       </c>
-      <c r="B57" s="16">
+      <c r="B57" s="12">
         <f t="shared" si="0"/>
         <v>0.3783783783783784</v>
       </c>
-      <c r="C57" s="14"/>
+      <c r="C57" s="18"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="2"/>
-      <c r="B58" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C58" s="14" t="s">
+      <c r="B58" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C58" s="18" t="s">
         <v>37</v>
       </c>
     </row>
@@ -3186,18 +4199,18 @@
       <c r="A59">
         <v>3.625</v>
       </c>
-      <c r="B59" s="16">
+      <c r="B59" s="12">
         <f t="shared" si="0"/>
         <v>0.39189189189189189</v>
       </c>
-      <c r="C59" s="14"/>
+      <c r="C59" s="18"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B60" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C60" s="14" t="s">
+      <c r="B60" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C60" s="18" t="s">
         <v>36</v>
       </c>
     </row>
@@ -3205,19 +4218,19 @@
       <c r="A61">
         <v>3.75</v>
       </c>
-      <c r="B61" s="16">
+      <c r="B61" s="12">
         <f t="shared" si="0"/>
         <v>0.40540540540540543</v>
       </c>
-      <c r="C61" s="14"/>
+      <c r="C61" s="18"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="2"/>
-      <c r="B62" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C62" s="14" t="s">
+      <c r="B62" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C62" s="18" t="s">
         <v>35</v>
       </c>
     </row>
@@ -3225,18 +4238,18 @@
       <c r="A63">
         <v>3.875</v>
       </c>
-      <c r="B63" s="16">
+      <c r="B63" s="12">
         <f t="shared" si="0"/>
         <v>0.41891891891891891</v>
       </c>
-      <c r="C63" s="14"/>
+      <c r="C63" s="18"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B64" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C64" s="14" t="s">
+      <c r="B64" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C64" s="18" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3244,87 +4257,87 @@
       <c r="A65">
         <v>4</v>
       </c>
-      <c r="B65" s="16">
+      <c r="B65" s="12">
         <f t="shared" si="0"/>
         <v>0.43243243243243246</v>
       </c>
-      <c r="C65" s="14"/>
+      <c r="C65" s="18"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="2"/>
-      <c r="B66" s="16" t="str">
+      <c r="B66" s="12" t="str">
         <f t="shared" ref="B66:B129" si="1">IF(NOT(ISBLANK(A66)), A66/9.25, "")</f>
         <v/>
       </c>
-      <c r="C66" s="14"/>
+      <c r="C66" s="18"/>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>4.125</v>
       </c>
-      <c r="B67" s="16">
+      <c r="B67" s="12">
         <f t="shared" si="1"/>
         <v>0.44594594594594594</v>
       </c>
-      <c r="C67" s="14"/>
+      <c r="C67" s="18"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B68" s="16" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C68" s="14"/>
+      <c r="B68" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C68" s="18"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>4.25</v>
       </c>
-      <c r="B69" s="16">
+      <c r="B69" s="12">
         <f t="shared" si="1"/>
         <v>0.45945945945945948</v>
       </c>
-      <c r="C69" s="14"/>
+      <c r="C69" s="18"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B70" s="16" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C70" s="14"/>
+      <c r="B70" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C70" s="18"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>4.375</v>
       </c>
-      <c r="B71" s="16">
+      <c r="B71" s="12">
         <f t="shared" si="1"/>
         <v>0.47297297297297297</v>
       </c>
-      <c r="C71" s="14"/>
+      <c r="C71" s="18"/>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B72" s="16" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C72" s="14"/>
+      <c r="B72" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C72" s="18"/>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>4.5</v>
       </c>
-      <c r="B73" s="16">
+      <c r="B73" s="12">
         <f t="shared" si="1"/>
         <v>0.48648648648648651</v>
       </c>
-      <c r="C73" s="14"/>
+      <c r="C73" s="18"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B74" s="16" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C74" s="14" t="s">
+      <c r="B74" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C74" s="18" t="s">
         <v>47</v>
       </c>
     </row>
@@ -3332,18 +4345,18 @@
       <c r="A75">
         <v>4.625</v>
       </c>
-      <c r="B75" s="16">
+      <c r="B75" s="12">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="C75" s="14"/>
+      <c r="C75" s="18"/>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B76" s="16" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C76" s="14" t="s">
+      <c r="B76" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C76" s="18" t="s">
         <v>38</v>
       </c>
     </row>
@@ -3351,18 +4364,18 @@
       <c r="A77">
         <v>4.75</v>
       </c>
-      <c r="B77" s="16">
+      <c r="B77" s="12">
         <f t="shared" si="1"/>
         <v>0.51351351351351349</v>
       </c>
-      <c r="C77" s="14"/>
+      <c r="C77" s="18"/>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B78" s="16" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C78" s="14" t="s">
+      <c r="B78" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C78" s="18" t="s">
         <v>48</v>
       </c>
     </row>
@@ -3370,18 +4383,18 @@
       <c r="A79">
         <v>4.875</v>
       </c>
-      <c r="B79" s="16">
+      <c r="B79" s="12">
         <f t="shared" si="1"/>
         <v>0.52702702702702697</v>
       </c>
-      <c r="C79" s="14"/>
+      <c r="C79" s="18"/>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B80" s="16" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C80" s="14" t="s">
+      <c r="B80" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C80" s="18" t="s">
         <v>49</v>
       </c>
     </row>
@@ -3389,18 +4402,18 @@
       <c r="A81">
         <v>5</v>
       </c>
-      <c r="B81" s="16">
+      <c r="B81" s="12">
         <f t="shared" si="1"/>
         <v>0.54054054054054057</v>
       </c>
-      <c r="C81" s="14"/>
+      <c r="C81" s="18"/>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B82" s="16" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C82" s="14" t="s">
+      <c r="B82" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C82" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -3408,18 +4421,18 @@
       <c r="A83">
         <v>5.125</v>
       </c>
-      <c r="B83" s="16">
+      <c r="B83" s="12">
         <f t="shared" si="1"/>
         <v>0.55405405405405406</v>
       </c>
-      <c r="C83" s="14"/>
+      <c r="C83" s="18"/>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B84" s="16" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C84" s="14" t="s">
+      <c r="B84" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C84" s="18" t="s">
         <v>36</v>
       </c>
     </row>
@@ -3427,18 +4440,18 @@
       <c r="A85">
         <v>5.25</v>
       </c>
-      <c r="B85" s="16">
+      <c r="B85" s="12">
         <f t="shared" si="1"/>
         <v>0.56756756756756754</v>
       </c>
-      <c r="C85" s="14"/>
+      <c r="C85" s="18"/>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B86" s="16" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C86" s="14" t="s">
+      <c r="B86" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C86" s="18" t="s">
         <v>37</v>
       </c>
     </row>
@@ -3446,18 +4459,18 @@
       <c r="A87">
         <v>5.375</v>
       </c>
-      <c r="B87" s="16">
+      <c r="B87" s="12">
         <f t="shared" si="1"/>
         <v>0.58108108108108103</v>
       </c>
-      <c r="C87" s="14"/>
+      <c r="C87" s="18"/>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B88" s="16" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C88" s="14" t="s">
+      <c r="B88" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C88" s="18" t="s">
         <v>42</v>
       </c>
     </row>
@@ -3465,18 +4478,18 @@
       <c r="A89">
         <v>5.5</v>
       </c>
-      <c r="B89" s="16">
+      <c r="B89" s="12">
         <f t="shared" si="1"/>
         <v>0.59459459459459463</v>
       </c>
-      <c r="C89" s="14"/>
+      <c r="C89" s="18"/>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B90" s="16" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C90" s="14" t="s">
+      <c r="B90" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C90" s="18" t="s">
         <v>43</v>
       </c>
     </row>
@@ -3484,18 +4497,18 @@
       <c r="A91">
         <v>5.625</v>
       </c>
-      <c r="B91" s="16">
+      <c r="B91" s="12">
         <f t="shared" si="1"/>
         <v>0.60810810810810811</v>
       </c>
-      <c r="C91" s="14"/>
+      <c r="C91" s="18"/>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B92" s="16" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C92" s="14" t="s">
+      <c r="B92" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C92" s="18" t="s">
         <v>46</v>
       </c>
     </row>
@@ -3503,18 +4516,18 @@
       <c r="A93">
         <v>5.75</v>
       </c>
-      <c r="B93" s="16">
+      <c r="B93" s="12">
         <f t="shared" si="1"/>
         <v>0.6216216216216216</v>
       </c>
-      <c r="C93" s="14"/>
+      <c r="C93" s="18"/>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B94" s="16" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C94" s="14" t="s">
+      <c r="B94" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C94" s="18" t="s">
         <v>41</v>
       </c>
     </row>
@@ -3522,18 +4535,18 @@
       <c r="A95">
         <v>5.875</v>
       </c>
-      <c r="B95" s="16">
+      <c r="B95" s="12">
         <f t="shared" si="1"/>
         <v>0.63513513513513509</v>
       </c>
-      <c r="C95" s="14"/>
+      <c r="C95" s="18"/>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B96" s="16" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C96" s="14" t="s">
+      <c r="B96" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C96" s="18" t="s">
         <v>51</v>
       </c>
     </row>
@@ -3541,18 +4554,18 @@
       <c r="A97">
         <v>6</v>
       </c>
-      <c r="B97" s="16">
+      <c r="B97" s="12">
         <f t="shared" si="1"/>
         <v>0.64864864864864868</v>
       </c>
-      <c r="C97" s="14"/>
+      <c r="C97" s="18"/>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B98" s="16" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C98" s="14" t="s">
+      <c r="B98" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C98" s="18" t="s">
         <v>40</v>
       </c>
     </row>
@@ -3560,18 +4573,18 @@
       <c r="A99">
         <v>6.125</v>
       </c>
-      <c r="B99" s="16">
+      <c r="B99" s="12">
         <f t="shared" si="1"/>
         <v>0.66216216216216217</v>
       </c>
-      <c r="C99" s="14"/>
+      <c r="C99" s="18"/>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B100" s="16" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C100" s="14" t="s">
+      <c r="B100" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C100" s="18" t="s">
         <v>41</v>
       </c>
     </row>
@@ -3579,18 +4592,18 @@
       <c r="A101">
         <v>6.25</v>
       </c>
-      <c r="B101" s="16">
+      <c r="B101" s="12">
         <f t="shared" si="1"/>
         <v>0.67567567567567566</v>
       </c>
-      <c r="C101" s="14"/>
+      <c r="C101" s="18"/>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B102" s="16" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C102" s="14" t="s">
+      <c r="B102" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C102" s="18" t="s">
         <v>42</v>
       </c>
     </row>
@@ -3598,18 +4611,18 @@
       <c r="A103">
         <v>6.375</v>
       </c>
-      <c r="B103" s="16">
+      <c r="B103" s="12">
         <f t="shared" si="1"/>
         <v>0.68918918918918914</v>
       </c>
-      <c r="C103" s="14"/>
+      <c r="C103" s="18"/>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B104" s="16" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C104" s="14" t="s">
+      <c r="B104" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C104" s="18" t="s">
         <v>42</v>
       </c>
     </row>
@@ -3617,18 +4630,18 @@
       <c r="A105">
         <v>6.5</v>
       </c>
-      <c r="B105" s="16">
+      <c r="B105" s="12">
         <f t="shared" si="1"/>
         <v>0.70270270270270274</v>
       </c>
-      <c r="C105" s="14"/>
+      <c r="C105" s="18"/>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B106" s="16" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C106" s="14" t="s">
+      <c r="B106" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C106" s="18" t="s">
         <v>37</v>
       </c>
     </row>
@@ -3636,86 +4649,86 @@
       <c r="A107">
         <v>6.625</v>
       </c>
-      <c r="B107" s="16">
+      <c r="B107" s="12">
         <f t="shared" si="1"/>
         <v>0.71621621621621623</v>
       </c>
-      <c r="C107" s="14"/>
+      <c r="C107" s="18"/>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B108" s="16" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C108" s="14"/>
+      <c r="B108" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C108" s="18"/>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>6.75</v>
       </c>
-      <c r="B109" s="16">
+      <c r="B109" s="12">
         <f t="shared" si="1"/>
         <v>0.72972972972972971</v>
       </c>
-      <c r="C109" s="14"/>
+      <c r="C109" s="18"/>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B110" s="16" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C110" s="14"/>
+      <c r="B110" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C110" s="18"/>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>6.875</v>
       </c>
-      <c r="B111" s="16">
+      <c r="B111" s="12">
         <f t="shared" si="1"/>
         <v>0.7432432432432432</v>
       </c>
-      <c r="C111" s="14"/>
+      <c r="C111" s="18"/>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B112" s="16" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C112" s="14"/>
+      <c r="B112" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C112" s="18"/>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>7</v>
       </c>
-      <c r="B113" s="16">
+      <c r="B113" s="12">
         <f t="shared" si="1"/>
         <v>0.7567567567567568</v>
       </c>
-      <c r="C113" s="14"/>
+      <c r="C113" s="18"/>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B114" s="16" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C114" s="14"/>
+      <c r="B114" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C114" s="18"/>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>7.125</v>
       </c>
-      <c r="B115" s="16">
+      <c r="B115" s="12">
         <f t="shared" si="1"/>
         <v>0.77027027027027029</v>
       </c>
-      <c r="C115" s="14"/>
+      <c r="C115" s="18"/>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B116" s="16" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C116" s="14" t="s">
+      <c r="B116" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C116" s="18" t="s">
         <v>42</v>
       </c>
     </row>
@@ -3723,18 +4736,18 @@
       <c r="A117">
         <v>7.25</v>
       </c>
-      <c r="B117" s="16">
+      <c r="B117" s="12">
         <f t="shared" si="1"/>
         <v>0.78378378378378377</v>
       </c>
-      <c r="C117" s="14"/>
+      <c r="C117" s="18"/>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B118" s="16" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C118" s="14" t="s">
+      <c r="B118" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C118" s="18" t="s">
         <v>42</v>
       </c>
     </row>
@@ -3742,18 +4755,18 @@
       <c r="A119">
         <v>7.375</v>
       </c>
-      <c r="B119" s="16">
+      <c r="B119" s="12">
         <f t="shared" si="1"/>
         <v>0.79729729729729726</v>
       </c>
-      <c r="C119" s="14"/>
+      <c r="C119" s="18"/>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B120" s="16" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C120" s="14" t="s">
+      <c r="B120" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C120" s="18" t="s">
         <v>41</v>
       </c>
     </row>
@@ -3761,18 +4774,18 @@
       <c r="A121">
         <v>7.5</v>
       </c>
-      <c r="B121" s="16">
+      <c r="B121" s="12">
         <f t="shared" si="1"/>
         <v>0.81081081081081086</v>
       </c>
-      <c r="C121" s="14"/>
+      <c r="C121" s="18"/>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B122" s="16" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C122" s="14" t="s">
+      <c r="B122" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C122" s="18" t="s">
         <v>40</v>
       </c>
     </row>
@@ -3780,18 +4793,18 @@
       <c r="A123">
         <v>7.625</v>
       </c>
-      <c r="B123" s="16">
+      <c r="B123" s="12">
         <f t="shared" si="1"/>
         <v>0.82432432432432434</v>
       </c>
-      <c r="C123" s="14"/>
+      <c r="C123" s="18"/>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B124" s="16" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C124" s="14" t="s">
+      <c r="B124" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C124" s="18" t="s">
         <v>51</v>
       </c>
     </row>
@@ -3799,18 +4812,18 @@
       <c r="A125">
         <v>7.75</v>
       </c>
-      <c r="B125" s="16">
+      <c r="B125" s="12">
         <f t="shared" si="1"/>
         <v>0.83783783783783783</v>
       </c>
-      <c r="C125" s="14"/>
+      <c r="C125" s="18"/>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B126" s="16" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C126" s="14" t="s">
+      <c r="B126" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C126" s="18" t="s">
         <v>41</v>
       </c>
     </row>
@@ -3818,18 +4831,18 @@
       <c r="A127">
         <v>7.875</v>
       </c>
-      <c r="B127" s="16">
+      <c r="B127" s="12">
         <f t="shared" si="1"/>
         <v>0.85135135135135132</v>
       </c>
-      <c r="C127" s="14"/>
+      <c r="C127" s="18"/>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B128" s="16" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C128" s="14" t="s">
+      <c r="B128" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C128" s="18" t="s">
         <v>46</v>
       </c>
     </row>
@@ -3837,18 +4850,18 @@
       <c r="A129">
         <v>8</v>
       </c>
-      <c r="B129" s="16">
+      <c r="B129" s="12">
         <f t="shared" si="1"/>
         <v>0.86486486486486491</v>
       </c>
-      <c r="C129" s="14"/>
+      <c r="C129" s="18"/>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B130" s="16" t="str">
+      <c r="B130" s="12" t="str">
         <f t="shared" ref="B130:B147" si="2">IF(NOT(ISBLANK(A130)), A130/9.25, "")</f>
         <v/>
       </c>
-      <c r="C130" s="14" t="s">
+      <c r="C130" s="18" t="s">
         <v>43</v>
       </c>
     </row>
@@ -3856,18 +4869,18 @@
       <c r="A131">
         <v>8.125</v>
       </c>
-      <c r="B131" s="16">
+      <c r="B131" s="12">
         <f t="shared" si="2"/>
         <v>0.8783783783783784</v>
       </c>
-      <c r="C131" s="14"/>
+      <c r="C131" s="18"/>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B132" s="16" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="C132" s="14" t="s">
+      <c r="B132" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="C132" s="18" t="s">
         <v>42</v>
       </c>
     </row>
@@ -3875,18 +4888,18 @@
       <c r="A133">
         <v>8.25</v>
       </c>
-      <c r="B133" s="16">
+      <c r="B133" s="12">
         <f t="shared" si="2"/>
         <v>0.89189189189189189</v>
       </c>
-      <c r="C133" s="14"/>
+      <c r="C133" s="18"/>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B134" s="16" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="C134" s="14" t="s">
+      <c r="B134" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="C134" s="18" t="s">
         <v>37</v>
       </c>
     </row>
@@ -3894,18 +4907,18 @@
       <c r="A135">
         <v>8.375</v>
       </c>
-      <c r="B135" s="16">
+      <c r="B135" s="12">
         <f t="shared" si="2"/>
         <v>0.90540540540540537</v>
       </c>
-      <c r="C135" s="14"/>
+      <c r="C135" s="18"/>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B136" s="16" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="C136" s="14" t="s">
+      <c r="B136" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="C136" s="18" t="s">
         <v>36</v>
       </c>
     </row>
@@ -3913,18 +4926,18 @@
       <c r="A137">
         <v>8.5</v>
       </c>
-      <c r="B137" s="16">
+      <c r="B137" s="12">
         <f t="shared" si="2"/>
         <v>0.91891891891891897</v>
       </c>
-      <c r="C137" s="14"/>
+      <c r="C137" s="18"/>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B138" s="16" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="C138" s="14" t="s">
+      <c r="B138" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="C138" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -3932,18 +4945,18 @@
       <c r="A139">
         <v>8.625</v>
       </c>
-      <c r="B139" s="16">
+      <c r="B139" s="12">
         <f t="shared" si="2"/>
         <v>0.93243243243243246</v>
       </c>
-      <c r="C139" s="14"/>
+      <c r="C139" s="18"/>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B140" s="16" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="C140" s="14" t="s">
+      <c r="B140" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="C140" s="18" t="s">
         <v>49</v>
       </c>
     </row>
@@ -3951,18 +4964,18 @@
       <c r="A141">
         <v>8.75</v>
       </c>
-      <c r="B141" s="16">
+      <c r="B141" s="12">
         <f t="shared" si="2"/>
         <v>0.94594594594594594</v>
       </c>
-      <c r="C141" s="14"/>
+      <c r="C141" s="18"/>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B142" s="16" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="C142" s="14" t="s">
+      <c r="B142" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="C142" s="18" t="s">
         <v>48</v>
       </c>
     </row>
@@ -3970,18 +4983,18 @@
       <c r="A143">
         <v>8.875</v>
       </c>
-      <c r="B143" s="16">
+      <c r="B143" s="12">
         <f t="shared" si="2"/>
         <v>0.95945945945945943</v>
       </c>
-      <c r="C143" s="14"/>
+      <c r="C143" s="18"/>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B144" s="16" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="C144" s="14" t="s">
+      <c r="B144" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="C144" s="18" t="s">
         <v>38</v>
       </c>
     </row>
@@ -3989,18 +5002,18 @@
       <c r="A145">
         <v>9</v>
       </c>
-      <c r="B145" s="16">
+      <c r="B145" s="12">
         <f t="shared" si="2"/>
         <v>0.97297297297297303</v>
       </c>
-      <c r="C145" s="14"/>
+      <c r="C145" s="18"/>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B146" s="16" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="C146" s="14" t="s">
+      <c r="B146" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="C146" s="18" t="s">
         <v>47</v>
       </c>
     </row>
@@ -4008,14 +5021,14 @@
       <c r="A147">
         <v>9.125</v>
       </c>
-      <c r="B147" s="16">
+      <c r="B147" s="12">
         <f t="shared" si="2"/>
         <v>0.98648648648648651</v>
       </c>
-      <c r="C147" s="14"/>
+      <c r="C147" s="18"/>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B148" s="16" t="str">
+      <c r="B148" s="12" t="str">
         <f>IF(NOT(ISBLANK(A148)), A148/9.25, "")</f>
         <v/>
       </c>
@@ -4024,386 +5037,342 @@
       <c r="A149">
         <v>9.25</v>
       </c>
-      <c r="B149" s="17">
+      <c r="B149" s="13">
         <f t="shared" ref="B149" si="3">IF(NOT(ISBLANK(A149)), A149/9.25, "")</f>
         <v>1</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B150" s="16"/>
+      <c r="B150" s="12"/>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B151" s="16"/>
+      <c r="B151" s="12"/>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B152" s="16"/>
+      <c r="B152" s="12"/>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B153" s="16"/>
+      <c r="B153" s="12"/>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B154" s="16"/>
+      <c r="B154" s="12"/>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B155" s="16"/>
+      <c r="B155" s="12"/>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B156" s="16"/>
+      <c r="B156" s="12"/>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B157" s="16"/>
+      <c r="B157" s="12"/>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B158" s="16"/>
+      <c r="B158" s="12"/>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B159" s="16"/>
+      <c r="B159" s="12"/>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B160" s="16"/>
+      <c r="B160" s="12"/>
     </row>
     <row r="161" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B161" s="16"/>
+      <c r="B161" s="12"/>
     </row>
     <row r="162" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B162" s="16"/>
+      <c r="B162" s="12"/>
     </row>
     <row r="163" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B163" s="16"/>
+      <c r="B163" s="12"/>
     </row>
     <row r="164" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B164" s="16"/>
+      <c r="B164" s="12"/>
     </row>
     <row r="165" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B165" s="16"/>
+      <c r="B165" s="12"/>
     </row>
     <row r="166" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B166" s="16"/>
+      <c r="B166" s="12"/>
     </row>
     <row r="167" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B167" s="16"/>
+      <c r="B167" s="12"/>
     </row>
     <row r="168" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B168" s="16"/>
+      <c r="B168" s="12"/>
     </row>
     <row r="169" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B169" s="16"/>
+      <c r="B169" s="12"/>
     </row>
     <row r="170" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B170" s="16"/>
+      <c r="B170" s="12"/>
     </row>
     <row r="171" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B171" s="16"/>
+      <c r="B171" s="12"/>
     </row>
     <row r="172" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B172" s="16"/>
+      <c r="B172" s="12"/>
     </row>
     <row r="173" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B173" s="16"/>
+      <c r="B173" s="12"/>
     </row>
     <row r="174" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B174" s="16"/>
+      <c r="B174" s="12"/>
     </row>
     <row r="175" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B175" s="16"/>
+      <c r="B175" s="12"/>
     </row>
     <row r="176" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B176" s="16"/>
+      <c r="B176" s="12"/>
     </row>
     <row r="177" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B177" s="16"/>
+      <c r="B177" s="12"/>
     </row>
     <row r="178" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B178" s="16"/>
+      <c r="B178" s="12"/>
     </row>
     <row r="179" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B179" s="16"/>
+      <c r="B179" s="12"/>
     </row>
     <row r="180" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B180" s="16"/>
+      <c r="B180" s="12"/>
     </row>
     <row r="181" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B181" s="16"/>
+      <c r="B181" s="12"/>
     </row>
     <row r="182" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B182" s="16"/>
+      <c r="B182" s="12"/>
     </row>
     <row r="183" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B183" s="16"/>
+      <c r="B183" s="12"/>
     </row>
     <row r="184" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B184" s="16"/>
+      <c r="B184" s="12"/>
     </row>
     <row r="185" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B185" s="16"/>
+      <c r="B185" s="12"/>
     </row>
     <row r="186" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B186" s="16"/>
+      <c r="B186" s="12"/>
     </row>
     <row r="187" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B187" s="16"/>
+      <c r="B187" s="12"/>
     </row>
     <row r="188" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B188" s="16"/>
+      <c r="B188" s="12"/>
     </row>
     <row r="189" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B189" s="16"/>
+      <c r="B189" s="12"/>
     </row>
     <row r="190" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B190" s="16"/>
+      <c r="B190" s="12"/>
     </row>
     <row r="191" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B191" s="16"/>
+      <c r="B191" s="12"/>
     </row>
     <row r="192" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B192" s="16"/>
+      <c r="B192" s="12"/>
     </row>
     <row r="193" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B193" s="16"/>
+      <c r="B193" s="12"/>
     </row>
     <row r="194" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B194" s="16"/>
+      <c r="B194" s="12"/>
     </row>
     <row r="195" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B195" s="16"/>
+      <c r="B195" s="12"/>
     </row>
     <row r="196" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B196" s="16"/>
+      <c r="B196" s="12"/>
     </row>
     <row r="197" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B197" s="16"/>
+      <c r="B197" s="12"/>
     </row>
     <row r="198" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B198" s="16"/>
+      <c r="B198" s="12"/>
     </row>
     <row r="199" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B199" s="16"/>
+      <c r="B199" s="12"/>
     </row>
     <row r="200" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B200" s="16"/>
+      <c r="B200" s="12"/>
     </row>
     <row r="201" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B201" s="16"/>
+      <c r="B201" s="12"/>
     </row>
     <row r="202" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B202" s="16"/>
+      <c r="B202" s="12"/>
     </row>
     <row r="203" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B203" s="16"/>
+      <c r="B203" s="12"/>
     </row>
     <row r="204" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B204" s="16"/>
+      <c r="B204" s="12"/>
     </row>
     <row r="205" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B205" s="16"/>
+      <c r="B205" s="12"/>
     </row>
     <row r="206" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B206" s="16"/>
+      <c r="B206" s="12"/>
     </row>
     <row r="207" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B207" s="16"/>
+      <c r="B207" s="12"/>
     </row>
     <row r="208" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B208" s="16"/>
+      <c r="B208" s="12"/>
     </row>
     <row r="209" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B209" s="16"/>
+      <c r="B209" s="12"/>
     </row>
     <row r="210" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B210" s="16"/>
+      <c r="B210" s="12"/>
     </row>
     <row r="211" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B211" s="16"/>
+      <c r="B211" s="12"/>
     </row>
     <row r="212" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B212" s="16"/>
+      <c r="B212" s="12"/>
     </row>
     <row r="213" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B213" s="16"/>
+      <c r="B213" s="12"/>
     </row>
     <row r="214" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B214" s="16"/>
+      <c r="B214" s="12"/>
     </row>
     <row r="215" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B215" s="16"/>
+      <c r="B215" s="12"/>
     </row>
     <row r="216" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B216" s="16"/>
+      <c r="B216" s="12"/>
     </row>
     <row r="217" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B217" s="16"/>
+      <c r="B217" s="12"/>
     </row>
     <row r="218" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B218" s="16"/>
+      <c r="B218" s="12"/>
     </row>
     <row r="219" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B219" s="16"/>
+      <c r="B219" s="12"/>
     </row>
     <row r="220" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B220" s="16"/>
+      <c r="B220" s="12"/>
     </row>
     <row r="221" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B221" s="16"/>
+      <c r="B221" s="12"/>
     </row>
     <row r="222" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B222" s="16"/>
+      <c r="B222" s="12"/>
     </row>
     <row r="223" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B223" s="16"/>
+      <c r="B223" s="12"/>
     </row>
     <row r="224" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B224" s="16"/>
+      <c r="B224" s="12"/>
     </row>
     <row r="225" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B225" s="16"/>
+      <c r="B225" s="12"/>
     </row>
     <row r="226" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B226" s="16"/>
+      <c r="B226" s="12"/>
     </row>
     <row r="227" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B227" s="16"/>
+      <c r="B227" s="12"/>
     </row>
     <row r="228" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B228" s="16"/>
+      <c r="B228" s="12"/>
     </row>
     <row r="229" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B229" s="16"/>
+      <c r="B229" s="12"/>
     </row>
     <row r="230" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B230" s="16"/>
+      <c r="B230" s="12"/>
     </row>
     <row r="231" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B231" s="16"/>
+      <c r="B231" s="12"/>
     </row>
     <row r="232" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B232" s="16"/>
+      <c r="B232" s="12"/>
     </row>
     <row r="233" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B233" s="16"/>
+      <c r="B233" s="12"/>
     </row>
     <row r="234" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B234" s="16"/>
+      <c r="B234" s="12"/>
     </row>
     <row r="235" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B235" s="16"/>
+      <c r="B235" s="12"/>
     </row>
     <row r="236" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B236" s="16"/>
+      <c r="B236" s="12"/>
     </row>
     <row r="237" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B237" s="16"/>
+      <c r="B237" s="12"/>
     </row>
     <row r="238" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B238" s="16"/>
+      <c r="B238" s="12"/>
     </row>
     <row r="239" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B239" s="16"/>
+      <c r="B239" s="12"/>
     </row>
     <row r="240" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B240" s="16"/>
+      <c r="B240" s="12"/>
     </row>
     <row r="241" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B241" s="16"/>
+      <c r="B241" s="12"/>
     </row>
     <row r="242" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B242" s="16"/>
+      <c r="B242" s="12"/>
     </row>
     <row r="243" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B243" s="16"/>
+      <c r="B243" s="12"/>
     </row>
     <row r="244" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B244" s="16"/>
+      <c r="B244" s="12"/>
     </row>
     <row r="245" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B245" s="16"/>
+      <c r="B245" s="12"/>
     </row>
     <row r="246" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B246" s="16"/>
+      <c r="B246" s="12"/>
     </row>
     <row r="247" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B247" s="16"/>
+      <c r="B247" s="12"/>
     </row>
     <row r="248" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B248" s="16"/>
+      <c r="B248" s="12"/>
     </row>
     <row r="249" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B249" s="16"/>
+      <c r="B249" s="12"/>
     </row>
     <row r="250" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B250" s="16"/>
+      <c r="B250" s="12"/>
     </row>
     <row r="251" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B251" s="16"/>
+      <c r="B251" s="12"/>
     </row>
     <row r="252" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B252" s="16"/>
+      <c r="B252" s="12"/>
     </row>
     <row r="253" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B253" s="16"/>
+      <c r="B253" s="12"/>
     </row>
     <row r="254" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B254" s="16"/>
+      <c r="B254" s="12"/>
     </row>
     <row r="255" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B255" s="16"/>
+      <c r="B255" s="12"/>
     </row>
     <row r="256" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B256" s="16"/>
+      <c r="B256" s="12"/>
     </row>
     <row r="257" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B257" s="16"/>
+      <c r="B257" s="12"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F2:F149">
     <sortCondition ref="F2:F149"/>
   </sortState>
   <mergeCells count="58">
-    <mergeCell ref="C136:C137"/>
-    <mergeCell ref="C138:C139"/>
-    <mergeCell ref="C140:C141"/>
-    <mergeCell ref="C142:C143"/>
-    <mergeCell ref="C144:C145"/>
-    <mergeCell ref="C146:C147"/>
-    <mergeCell ref="C124:C125"/>
-    <mergeCell ref="C126:C127"/>
-    <mergeCell ref="C128:C129"/>
-    <mergeCell ref="C130:C131"/>
-    <mergeCell ref="C132:C133"/>
-    <mergeCell ref="C134:C135"/>
-    <mergeCell ref="C106:C115"/>
-    <mergeCell ref="C116:C117"/>
-    <mergeCell ref="C118:C119"/>
-    <mergeCell ref="C120:C121"/>
-    <mergeCell ref="C122:C123"/>
-    <mergeCell ref="C94:C95"/>
-    <mergeCell ref="C96:C97"/>
-    <mergeCell ref="C98:C99"/>
-    <mergeCell ref="C100:C101"/>
-    <mergeCell ref="C102:C103"/>
-    <mergeCell ref="C104:C105"/>
-    <mergeCell ref="C82:C83"/>
-    <mergeCell ref="C84:C85"/>
-    <mergeCell ref="C86:C87"/>
-    <mergeCell ref="C88:C89"/>
-    <mergeCell ref="C90:C91"/>
-    <mergeCell ref="C92:C93"/>
-    <mergeCell ref="C74:C75"/>
-    <mergeCell ref="C76:C77"/>
-    <mergeCell ref="C32:C41"/>
-    <mergeCell ref="C64:C73"/>
-    <mergeCell ref="C78:C79"/>
-    <mergeCell ref="C80:C81"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="C62:C63"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="C1:C9"/>
+    <mergeCell ref="C10:C11"/>
     <mergeCell ref="C24:C25"/>
     <mergeCell ref="C26:C27"/>
     <mergeCell ref="C28:C29"/>
@@ -4414,8 +5383,52 @@
     <mergeCell ref="C18:C19"/>
     <mergeCell ref="C20:C21"/>
     <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C1:C9"/>
-    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C80:C81"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="C74:C75"/>
+    <mergeCell ref="C76:C77"/>
+    <mergeCell ref="C32:C41"/>
+    <mergeCell ref="C64:C73"/>
+    <mergeCell ref="C78:C79"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="C104:C105"/>
+    <mergeCell ref="C82:C83"/>
+    <mergeCell ref="C84:C85"/>
+    <mergeCell ref="C86:C87"/>
+    <mergeCell ref="C88:C89"/>
+    <mergeCell ref="C90:C91"/>
+    <mergeCell ref="C92:C93"/>
+    <mergeCell ref="C94:C95"/>
+    <mergeCell ref="C96:C97"/>
+    <mergeCell ref="C98:C99"/>
+    <mergeCell ref="C100:C101"/>
+    <mergeCell ref="C102:C103"/>
+    <mergeCell ref="C106:C115"/>
+    <mergeCell ref="C116:C117"/>
+    <mergeCell ref="C118:C119"/>
+    <mergeCell ref="C120:C121"/>
+    <mergeCell ref="C122:C123"/>
+    <mergeCell ref="C146:C147"/>
+    <mergeCell ref="C124:C125"/>
+    <mergeCell ref="C126:C127"/>
+    <mergeCell ref="C128:C129"/>
+    <mergeCell ref="C130:C131"/>
+    <mergeCell ref="C132:C133"/>
+    <mergeCell ref="C134:C135"/>
+    <mergeCell ref="C136:C137"/>
+    <mergeCell ref="C138:C139"/>
+    <mergeCell ref="C140:C141"/>
+    <mergeCell ref="C142:C143"/>
+    <mergeCell ref="C144:C145"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>